<commit_message>
update table design with sample data
</commit_message>
<xml_diff>
--- a/doc/BLOG_TABLE_Design.xlsx
+++ b/doc/BLOG_TABLE_Design.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="101">
   <si>
     <t>Table Information</t>
   </si>
@@ -324,6 +324,9 @@
   </si>
   <si>
     <t>My name is Vy. Please contact me by ….</t>
+  </si>
+  <si>
+    <t>id(pk)</t>
   </si>
 </sst>
 </file>
@@ -409,7 +412,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -422,6 +425,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="35">
     <border>
@@ -884,7 +893,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -904,16 +913,7 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -922,19 +922,200 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -967,186 +1148,23 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="22" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="22" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1164,6 +1182,240 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>114</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>118</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="2352675" y="20288250"/>
+          <a:ext cx="1990725" cy="609601"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>962025</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>133351</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>126</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3305175" y="21107401"/>
+          <a:ext cx="1028700" cy="1009649"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>114</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>460344</xdr:colOff>
+      <xdr:row>132</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="Straight Connector 23"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="666750" y="20297775"/>
+          <a:ext cx="41244" cy="2667001"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>131</xdr:row>
+      <xdr:rowOff>114301</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>131</xdr:row>
+      <xdr:rowOff>140422</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="28" name="Straight Connector 27"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="647700" y="22917151"/>
+          <a:ext cx="1724025" cy="26121"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>114</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>114</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="35" name="Straight Arrow Connector 34"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="695325" y="20297775"/>
+          <a:ext cx="695325" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1429,10 +1681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q102"/>
+  <dimension ref="A1:Q133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="K88" sqref="K88"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="F128" sqref="F128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -1440,8 +1692,8 @@
     <col min="1" max="1" width="3.7109375" style="4" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" style="2" customWidth="1"/>
     <col min="3" max="4" width="14.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" style="3" customWidth="1"/>
     <col min="7" max="7" width="28.7109375" style="2" customWidth="1"/>
     <col min="8" max="9" width="8.85546875" style="4"/>
     <col min="10" max="10" width="18.7109375" style="4" customWidth="1"/>
@@ -1463,101 +1715,101 @@
       <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="86" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="9" t="s">
+      <c r="D2" s="87"/>
+      <c r="E2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="86" t="s">
         <v>39</v>
       </c>
-      <c r="G2" s="10"/>
+      <c r="G2" s="88"/>
     </row>
     <row r="3" spans="1:17" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="14" t="s">
+      <c r="C3" s="73"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="89" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="16"/>
+      <c r="G3" s="75"/>
     </row>
     <row r="4" spans="1:17" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="14" t="s">
+      <c r="C4" s="73"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="16"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="75"/>
     </row>
     <row r="5" spans="1:17" ht="24" x14ac:dyDescent="0.25">
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="16"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="75"/>
     </row>
     <row r="6" spans="1:17" ht="24" x14ac:dyDescent="0.25">
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="73" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="16"/>
+      <c r="D6" s="74"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="73"/>
+      <c r="G6" s="75"/>
     </row>
     <row r="7" spans="1:17" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="20"/>
+      <c r="C7" s="77"/>
+      <c r="D7" s="77"/>
+      <c r="E7" s="77"/>
+      <c r="F7" s="77"/>
+      <c r="G7" s="78"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="21"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="23"/>
+      <c r="B8" s="79"/>
+      <c r="C8" s="80"/>
+      <c r="D8" s="80"/>
+      <c r="E8" s="80"/>
+      <c r="F8" s="80"/>
+      <c r="G8" s="81"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="24"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="23"/>
+      <c r="B9" s="82"/>
+      <c r="C9" s="80"/>
+      <c r="D9" s="80"/>
+      <c r="E9" s="80"/>
+      <c r="F9" s="80"/>
+      <c r="G9" s="81"/>
     </row>
     <row r="10" spans="1:17" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="25"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="27"/>
+      <c r="B10" s="83"/>
+      <c r="C10" s="84"/>
+      <c r="D10" s="84"/>
+      <c r="E10" s="84"/>
+      <c r="F10" s="84"/>
+      <c r="G10" s="85"/>
     </row>
     <row r="12" spans="1:17" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
@@ -1568,94 +1820,94 @@
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="29" t="s">
+      <c r="C13" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="29" t="s">
+      <c r="D13" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="30" t="s">
+      <c r="E13" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="29" t="s">
+      <c r="F13" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="31" t="s">
+      <c r="G13" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I13" s="83" t="s">
+      <c r="I13" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="J13" s="32" t="s">
+      <c r="J13" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="K13" s="32" t="s">
+      <c r="K13" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="L13" s="32" t="s">
+      <c r="L13" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="M13" s="33" t="s">
+      <c r="M13" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="N13" s="32" t="s">
+      <c r="N13" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="O13" s="32" t="s">
+      <c r="O13" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="P13" s="32" t="s">
+      <c r="P13" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="Q13" s="32" t="s">
+      <c r="Q13" s="16" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="15" x14ac:dyDescent="0.2">
-      <c r="A14" s="34">
+      <c r="A14" s="18">
         <v>1</v>
       </c>
-      <c r="B14" s="35" t="s">
+      <c r="B14" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="36" t="s">
+      <c r="C14" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="35" t="s">
+      <c r="D14" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="37" t="s">
+      <c r="E14" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="38"/>
-      <c r="G14" s="39" t="s">
+      <c r="F14" s="22"/>
+      <c r="G14" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="I14" s="84">
+      <c r="I14" s="59">
         <v>1</v>
       </c>
       <c r="J14" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="K14" s="80" t="s">
+      <c r="K14" s="55" t="s">
         <v>63</v>
       </c>
-      <c r="L14" s="81" t="s">
+      <c r="L14" s="56" t="s">
         <v>64</v>
       </c>
       <c r="M14" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="N14" s="40" t="s">
+      <c r="N14" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="O14" s="82">
+      <c r="O14" s="57">
         <v>1415962923</v>
       </c>
       <c r="P14" s="4" t="s">
@@ -1666,24 +1918,24 @@
       </c>
     </row>
     <row r="15" spans="1:17" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="41">
+      <c r="A15" s="25">
         <v>2</v>
       </c>
-      <c r="B15" s="42" t="s">
+      <c r="B15" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="43" t="s">
+      <c r="C15" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="44" t="s">
+      <c r="D15" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="45" t="s">
+      <c r="E15" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="F15" s="46"/>
-      <c r="G15" s="47"/>
-      <c r="I15" s="84">
+      <c r="F15" s="30"/>
+      <c r="G15" s="31"/>
+      <c r="I15" s="59">
         <v>2</v>
       </c>
       <c r="J15" s="4" t="s">
@@ -1692,16 +1944,16 @@
       <c r="K15" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="L15" s="81" t="s">
+      <c r="L15" s="56" t="s">
         <v>69</v>
       </c>
       <c r="M15" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="N15" s="40" t="s">
+      <c r="N15" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="O15" s="82">
+      <c r="O15" s="57">
         <v>1415962923</v>
       </c>
       <c r="P15" s="4" t="s">
@@ -1712,226 +1964,226 @@
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="41">
+      <c r="A16" s="25">
         <f t="shared" ref="A16:A20" si="0">A15+1</f>
         <v>3</v>
       </c>
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="44" t="s">
+      <c r="C16" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="44" t="s">
+      <c r="D16" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="E16" s="45" t="s">
+      <c r="E16" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="F16" s="46"/>
-      <c r="G16" s="47"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="31"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="41">
+      <c r="A17" s="25">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B17" s="42" t="s">
+      <c r="B17" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="44" t="s">
+      <c r="C17" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="44" t="s">
+      <c r="D17" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="E17" s="45" t="s">
+      <c r="E17" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="F17" s="46"/>
-      <c r="G17" s="47"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="31"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="41">
+      <c r="A18" s="25">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="44" t="s">
+      <c r="C18" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="D18" s="44" t="s">
+      <c r="D18" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="45" t="s">
+      <c r="E18" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="F18" s="46"/>
-      <c r="G18" s="47"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="31"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="41">
+      <c r="A19" s="25">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B19" s="42" t="s">
+      <c r="B19" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="44" t="s">
+      <c r="C19" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="D19" s="44" t="s">
+      <c r="D19" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="E19" s="45" t="s">
+      <c r="E19" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="F19" s="46"/>
-      <c r="G19" s="47"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="31"/>
     </row>
     <row r="20" spans="1:15" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="48">
+      <c r="A20" s="32">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B20" s="49" t="s">
+      <c r="B20" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="C20" s="50" t="s">
+      <c r="C20" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="D20" s="51" t="s">
+      <c r="D20" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="E20" s="52" t="s">
+      <c r="E20" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="53" t="s">
+      <c r="F20" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="G20" s="54" t="s">
+      <c r="G20" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="N20" s="40"/>
-      <c r="O20" s="40"/>
+      <c r="N20" s="24"/>
+      <c r="O20" s="24"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="N21" s="40"/>
-      <c r="O21" s="40"/>
+      <c r="N21" s="24"/>
+      <c r="O21" s="24"/>
     </row>
     <row r="22" spans="1:15" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I22" s="71"/>
-      <c r="J22" s="71"/>
-      <c r="K22" s="71"/>
-      <c r="L22" s="71"/>
-      <c r="M22" s="72"/>
-      <c r="N22" s="73"/>
-      <c r="O22" s="73"/>
+      <c r="I22" s="49"/>
+      <c r="J22" s="49"/>
+      <c r="K22" s="49"/>
+      <c r="L22" s="49"/>
+      <c r="M22" s="50"/>
+      <c r="N22" s="51"/>
+      <c r="O22" s="51"/>
     </row>
     <row r="23" spans="1:15" ht="24" x14ac:dyDescent="0.25">
-      <c r="A23" s="55" t="s">
+      <c r="A23" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="56" t="s">
+      <c r="B23" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="57" t="s">
+      <c r="C23" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="58"/>
-      <c r="E23" s="56" t="s">
+      <c r="D23" s="65"/>
+      <c r="E23" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="F23" s="56" t="s">
+      <c r="F23" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="G23" s="59" t="s">
+      <c r="G23" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="I23" s="71"/>
-      <c r="J23" s="71"/>
-      <c r="K23" s="71"/>
-      <c r="L23" s="71"/>
-      <c r="M23" s="72"/>
-      <c r="N23" s="73"/>
-      <c r="O23" s="73"/>
+      <c r="I23" s="49"/>
+      <c r="J23" s="49"/>
+      <c r="K23" s="49"/>
+      <c r="L23" s="49"/>
+      <c r="M23" s="50"/>
+      <c r="N23" s="51"/>
+      <c r="O23" s="51"/>
     </row>
     <row r="24" spans="1:15" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A24" s="60">
+      <c r="A24" s="42">
         <v>1</v>
       </c>
-      <c r="B24" s="61" t="s">
+      <c r="B24" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="62" t="s">
+      <c r="C24" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="63"/>
-      <c r="E24" s="64" t="s">
+      <c r="D24" s="67"/>
+      <c r="E24" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="F24" s="64" t="s">
+      <c r="F24" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="G24" s="65"/>
-      <c r="I24" s="71"/>
-      <c r="J24" s="71"/>
-      <c r="K24" s="71"/>
-      <c r="L24" s="71"/>
-      <c r="M24" s="72"/>
-      <c r="N24" s="73"/>
-      <c r="O24" s="73"/>
+      <c r="G24" s="45"/>
+      <c r="I24" s="49"/>
+      <c r="J24" s="49"/>
+      <c r="K24" s="49"/>
+      <c r="L24" s="49"/>
+      <c r="M24" s="50"/>
+      <c r="N24" s="51"/>
+      <c r="O24" s="51"/>
     </row>
     <row r="25" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="66">
+      <c r="A25" s="46">
         <v>2</v>
       </c>
-      <c r="B25" s="51"/>
-      <c r="C25" s="67"/>
-      <c r="D25" s="68"/>
-      <c r="E25" s="69"/>
-      <c r="F25" s="69"/>
-      <c r="G25" s="70"/>
-      <c r="I25" s="71"/>
-      <c r="J25" s="71"/>
-      <c r="K25" s="71"/>
-      <c r="L25" s="71"/>
-      <c r="M25" s="72"/>
-      <c r="N25" s="73"/>
-      <c r="O25" s="73"/>
+      <c r="B25" s="35"/>
+      <c r="C25" s="68"/>
+      <c r="D25" s="69"/>
+      <c r="E25" s="47"/>
+      <c r="F25" s="47"/>
+      <c r="G25" s="48"/>
+      <c r="I25" s="49"/>
+      <c r="J25" s="49"/>
+      <c r="K25" s="49"/>
+      <c r="L25" s="49"/>
+      <c r="M25" s="50"/>
+      <c r="N25" s="51"/>
+      <c r="O25" s="51"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="N26" s="40"/>
-      <c r="O26" s="40"/>
+      <c r="N26" s="24"/>
+      <c r="O26" s="24"/>
     </row>
     <row r="27" spans="1:15" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="N27" s="40"/>
-      <c r="O27" s="40"/>
+      <c r="N27" s="24"/>
+      <c r="O27" s="24"/>
     </row>
     <row r="28" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="74" t="s">
+      <c r="A28" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="75" t="s">
+      <c r="B28" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="C28" s="76" t="s">
+      <c r="C28" s="70" t="s">
         <v>27</v>
       </c>
-      <c r="D28" s="77"/>
-      <c r="E28" s="76" t="s">
+      <c r="D28" s="71"/>
+      <c r="E28" s="70" t="s">
         <v>33</v>
       </c>
-      <c r="F28" s="78"/>
-      <c r="G28" s="79" t="s">
+      <c r="F28" s="72"/>
+      <c r="G28" s="54" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1941,21 +2193,21 @@
       </c>
     </row>
     <row r="31" spans="1:15" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="74" t="s">
+      <c r="A31" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="B31" s="75" t="s">
+      <c r="B31" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="C31" s="76" t="s">
+      <c r="C31" s="70" t="s">
         <v>27</v>
       </c>
-      <c r="D31" s="77"/>
-      <c r="E31" s="76" t="s">
+      <c r="D31" s="71"/>
+      <c r="E31" s="70" t="s">
         <v>36</v>
       </c>
-      <c r="F31" s="78"/>
-      <c r="G31" s="79" t="s">
+      <c r="F31" s="72"/>
+      <c r="G31" s="54" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1968,101 +2220,101 @@
       <c r="B37" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C37" s="86" t="s">
         <v>38</v>
       </c>
-      <c r="D37" s="8"/>
-      <c r="E37" s="9" t="s">
+      <c r="D37" s="87"/>
+      <c r="E37" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F37" s="7" t="s">
+      <c r="F37" s="86" t="s">
         <v>39</v>
       </c>
-      <c r="G37" s="10"/>
+      <c r="G37" s="88"/>
     </row>
     <row r="38" spans="1:15" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="B38" s="11" t="s">
+      <c r="B38" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C38" s="12"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="14" t="s">
+      <c r="C38" s="73"/>
+      <c r="D38" s="74"/>
+      <c r="E38" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F38" s="15" t="s">
+      <c r="F38" s="89" t="s">
         <v>40</v>
       </c>
-      <c r="G38" s="16"/>
+      <c r="G38" s="75"/>
     </row>
     <row r="39" spans="1:15" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="B39" s="11" t="s">
+      <c r="B39" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C39" s="12"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="14" t="s">
+      <c r="C39" s="73"/>
+      <c r="D39" s="74"/>
+      <c r="E39" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F39" s="12"/>
-      <c r="G39" s="16"/>
+      <c r="F39" s="73"/>
+      <c r="G39" s="75"/>
     </row>
     <row r="40" spans="1:15" ht="24" x14ac:dyDescent="0.25">
-      <c r="B40" s="11" t="s">
+      <c r="B40" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C40" s="12" t="s">
+      <c r="C40" s="73" t="s">
         <v>71</v>
       </c>
-      <c r="D40" s="13"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="12"/>
-      <c r="G40" s="16"/>
+      <c r="D40" s="74"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="73"/>
+      <c r="G40" s="75"/>
     </row>
     <row r="41" spans="1:15" ht="24" x14ac:dyDescent="0.25">
-      <c r="B41" s="11" t="s">
+      <c r="B41" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C41" s="12" t="s">
+      <c r="C41" s="73" t="s">
         <v>72</v>
       </c>
-      <c r="D41" s="13"/>
-      <c r="E41" s="17"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="16"/>
+      <c r="D41" s="74"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="73"/>
+      <c r="G41" s="75"/>
     </row>
     <row r="42" spans="1:15" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="B42" s="18" t="s">
+      <c r="B42" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19"/>
-      <c r="G42" s="20"/>
+      <c r="C42" s="77"/>
+      <c r="D42" s="77"/>
+      <c r="E42" s="77"/>
+      <c r="F42" s="77"/>
+      <c r="G42" s="78"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B43" s="21"/>
-      <c r="C43" s="22"/>
-      <c r="D43" s="22"/>
-      <c r="E43" s="22"/>
-      <c r="F43" s="22"/>
-      <c r="G43" s="23"/>
+      <c r="B43" s="79"/>
+      <c r="C43" s="80"/>
+      <c r="D43" s="80"/>
+      <c r="E43" s="80"/>
+      <c r="F43" s="80"/>
+      <c r="G43" s="81"/>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B44" s="24"/>
-      <c r="C44" s="22"/>
-      <c r="D44" s="22"/>
-      <c r="E44" s="22"/>
-      <c r="F44" s="22"/>
-      <c r="G44" s="23"/>
+      <c r="B44" s="82"/>
+      <c r="C44" s="80"/>
+      <c r="D44" s="80"/>
+      <c r="E44" s="80"/>
+      <c r="F44" s="80"/>
+      <c r="G44" s="81"/>
     </row>
     <row r="45" spans="1:15" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="25"/>
-      <c r="C45" s="26"/>
-      <c r="D45" s="26"/>
-      <c r="E45" s="26"/>
-      <c r="F45" s="26"/>
-      <c r="G45" s="27"/>
+      <c r="B45" s="83"/>
+      <c r="C45" s="84"/>
+      <c r="D45" s="84"/>
+      <c r="E45" s="84"/>
+      <c r="F45" s="84"/>
+      <c r="G45" s="85"/>
     </row>
     <row r="47" spans="1:15" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
@@ -2073,70 +2325,70 @@
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A48" s="28" t="s">
+      <c r="A48" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B48" s="29" t="s">
+      <c r="B48" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C48" s="29" t="s">
+      <c r="C48" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D48" s="29" t="s">
+      <c r="D48" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E48" s="30" t="s">
+      <c r="E48" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F48" s="29" t="s">
+      <c r="F48" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G48" s="31" t="s">
+      <c r="G48" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I48" s="83" t="s">
+      <c r="I48" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="J48" s="32" t="s">
+      <c r="J48" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="K48" s="32" t="s">
+      <c r="K48" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="L48" s="32" t="s">
+      <c r="L48" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="M48" s="33" t="s">
+      <c r="M48" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="N48" s="32" t="s">
+      <c r="N48" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="O48" s="32" t="s">
+      <c r="O48" s="16" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="49" spans="1:15" ht="24" x14ac:dyDescent="0.25">
-      <c r="A49" s="85">
+      <c r="A49" s="60">
         <v>1</v>
       </c>
-      <c r="B49" s="87" t="s">
+      <c r="B49" s="62" t="s">
         <v>74</v>
       </c>
-      <c r="C49" s="87" t="s">
+      <c r="C49" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="D49" s="87" t="s">
+      <c r="D49" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="E49" s="86" t="s">
+      <c r="E49" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="F49" s="87"/>
-      <c r="G49" s="39" t="s">
+      <c r="F49" s="62"/>
+      <c r="G49" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="I49" s="84">
+      <c r="I49" s="59">
         <v>1</v>
       </c>
       <c r="J49" s="4" t="s">
@@ -2145,10 +2397,10 @@
       <c r="K49" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="L49" s="82">
+      <c r="L49" s="57">
         <v>1415962923</v>
       </c>
-      <c r="M49" s="82">
+      <c r="M49" s="57">
         <v>1415962923</v>
       </c>
       <c r="N49" s="4">
@@ -2159,7 +2411,7 @@
       </c>
     </row>
     <row r="50" spans="1:15" ht="24" x14ac:dyDescent="0.25">
-      <c r="A50" s="34">
+      <c r="A50" s="18">
         <v>2</v>
       </c>
       <c r="B50" s="4" t="s">
@@ -2171,12 +2423,12 @@
       <c r="D50" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E50" s="84" t="s">
+      <c r="E50" s="59" t="s">
         <v>21</v>
       </c>
       <c r="F50" s="4"/>
       <c r="G50" s="4"/>
-      <c r="I50" s="84">
+      <c r="I50" s="59">
         <v>2</v>
       </c>
       <c r="J50" s="4" t="s">
@@ -2185,10 +2437,10 @@
       <c r="K50" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="L50" s="82">
+      <c r="L50" s="57">
         <v>1415962923</v>
       </c>
-      <c r="M50" s="82">
+      <c r="M50" s="57">
         <v>1415962923</v>
       </c>
       <c r="N50" s="4">
@@ -2199,108 +2451,108 @@
       </c>
     </row>
     <row r="51" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A51" s="85">
+      <c r="A51" s="60">
         <v>3</v>
       </c>
-      <c r="B51" s="42" t="s">
+      <c r="B51" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="C51" s="43" t="s">
+      <c r="C51" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="D51" s="44" t="s">
+      <c r="D51" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="E51" s="45" t="s">
+      <c r="E51" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="F51" s="46"/>
-      <c r="G51" s="47"/>
-      <c r="I51" s="84"/>
-      <c r="L51" s="88"/>
+      <c r="F51" s="30"/>
+      <c r="G51" s="31"/>
+      <c r="I51" s="59"/>
+      <c r="L51" s="63"/>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A52" s="34">
+      <c r="A52" s="18">
         <v>4</v>
       </c>
-      <c r="B52" s="42" t="s">
+      <c r="B52" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="C52" s="44" t="s">
+      <c r="C52" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="D52" s="44" t="s">
+      <c r="D52" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="E52" s="45" t="s">
+      <c r="E52" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="F52" s="46"/>
-      <c r="G52" s="47"/>
+      <c r="F52" s="30"/>
+      <c r="G52" s="31"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A53" s="85">
+      <c r="A53" s="60">
         <v>5</v>
       </c>
-      <c r="B53" s="42" t="s">
+      <c r="B53" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="C53" s="44" t="s">
+      <c r="C53" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="D53" s="44" t="s">
+      <c r="D53" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="E53" s="45" t="s">
+      <c r="E53" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="F53" s="46"/>
-      <c r="G53" s="47"/>
+      <c r="F53" s="30"/>
+      <c r="G53" s="31"/>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A54" s="34">
+      <c r="A54" s="18">
         <v>6</v>
       </c>
-      <c r="B54" s="42" t="s">
+      <c r="B54" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="C54" s="44" t="s">
+      <c r="C54" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="D54" s="44" t="s">
+      <c r="D54" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="E54" s="45" t="s">
+      <c r="E54" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="F54" s="46"/>
-      <c r="G54" s="47"/>
-      <c r="I54" s="35"/>
-      <c r="J54" s="36"/>
-      <c r="K54" s="35"/>
-      <c r="L54" s="37"/>
-      <c r="M54" s="38"/>
+      <c r="F54" s="30"/>
+      <c r="G54" s="31"/>
+      <c r="I54" s="19"/>
+      <c r="J54" s="20"/>
+      <c r="K54" s="19"/>
+      <c r="L54" s="21"/>
+      <c r="M54" s="22"/>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A55" s="85">
+      <c r="A55" s="60">
         <v>7</v>
       </c>
-      <c r="B55" s="42" t="s">
+      <c r="B55" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="C55" s="44" t="s">
+      <c r="C55" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="D55" s="44" t="s">
+      <c r="D55" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="E55" s="45" t="s">
+      <c r="E55" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="F55" s="46" t="s">
+      <c r="F55" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="G55" s="47" t="s">
+      <c r="G55" s="31" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2310,73 +2562,73 @@
       </c>
     </row>
     <row r="58" spans="1:15" ht="24" x14ac:dyDescent="0.25">
-      <c r="A58" s="55" t="s">
+      <c r="A58" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="B58" s="56" t="s">
+      <c r="B58" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="C58" s="57" t="s">
+      <c r="C58" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="D58" s="58"/>
-      <c r="E58" s="56" t="s">
+      <c r="D58" s="65"/>
+      <c r="E58" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="F58" s="56" t="s">
+      <c r="F58" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="G58" s="59" t="s">
+      <c r="G58" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="I58" s="71"/>
-      <c r="J58" s="71"/>
-      <c r="K58" s="71"/>
-      <c r="L58" s="71"/>
+      <c r="I58" s="49"/>
+      <c r="J58" s="49"/>
+      <c r="K58" s="49"/>
+      <c r="L58" s="49"/>
     </row>
     <row r="59" spans="1:15" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A59" s="60">
+      <c r="A59" s="42">
         <v>1</v>
       </c>
-      <c r="B59" s="61" t="s">
+      <c r="B59" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="C59" s="62" t="s">
+      <c r="C59" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="D59" s="63"/>
-      <c r="E59" s="64" t="s">
+      <c r="D59" s="67"/>
+      <c r="E59" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="F59" s="64" t="s">
+      <c r="F59" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="G59" s="65"/>
-      <c r="I59" s="71"/>
-      <c r="J59" s="71"/>
-      <c r="K59" s="71"/>
-      <c r="L59" s="71"/>
+      <c r="G59" s="45"/>
+      <c r="I59" s="49"/>
+      <c r="J59" s="49"/>
+      <c r="K59" s="49"/>
+      <c r="L59" s="49"/>
     </row>
     <row r="60" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="66">
+      <c r="A60" s="46">
         <v>2</v>
       </c>
-      <c r="B60" s="51"/>
-      <c r="C60" s="67"/>
-      <c r="D60" s="68"/>
-      <c r="E60" s="69"/>
-      <c r="F60" s="69"/>
-      <c r="G60" s="70"/>
-      <c r="I60" s="71"/>
-      <c r="J60" s="71"/>
-      <c r="K60" s="71"/>
-      <c r="L60" s="71"/>
+      <c r="B60" s="35"/>
+      <c r="C60" s="68"/>
+      <c r="D60" s="69"/>
+      <c r="E60" s="47"/>
+      <c r="F60" s="47"/>
+      <c r="G60" s="48"/>
+      <c r="I60" s="49"/>
+      <c r="J60" s="49"/>
+      <c r="K60" s="49"/>
+      <c r="L60" s="49"/>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I61" s="71"/>
-      <c r="J61" s="71"/>
-      <c r="K61" s="71"/>
-      <c r="L61" s="71"/>
+      <c r="I61" s="49"/>
+      <c r="J61" s="49"/>
+      <c r="K61" s="49"/>
+      <c r="L61" s="49"/>
     </row>
     <row r="62" spans="1:15" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
@@ -2384,21 +2636,21 @@
       </c>
     </row>
     <row r="63" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="74" t="s">
+      <c r="A63" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="B63" s="75" t="s">
+      <c r="B63" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="C63" s="76" t="s">
+      <c r="C63" s="70" t="s">
         <v>27</v>
       </c>
-      <c r="D63" s="77"/>
-      <c r="E63" s="76" t="s">
+      <c r="D63" s="71"/>
+      <c r="E63" s="70" t="s">
         <v>33</v>
       </c>
-      <c r="F63" s="78"/>
-      <c r="G63" s="79" t="s">
+      <c r="F63" s="72"/>
+      <c r="G63" s="54" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2422,21 +2674,21 @@
       </c>
     </row>
     <row r="67" spans="1:7" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="74" t="s">
+      <c r="A67" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="B67" s="75" t="s">
+      <c r="B67" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="C67" s="76" t="s">
+      <c r="C67" s="70" t="s">
         <v>27</v>
       </c>
-      <c r="D67" s="77"/>
-      <c r="E67" s="76" t="s">
+      <c r="D67" s="71"/>
+      <c r="E67" s="70" t="s">
         <v>36</v>
       </c>
-      <c r="F67" s="77"/>
-      <c r="G67" s="79" t="s">
+      <c r="F67" s="71"/>
+      <c r="G67" s="54" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2449,101 +2701,101 @@
       <c r="B73" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C73" s="7" t="s">
+      <c r="C73" s="86" t="s">
         <v>38</v>
       </c>
-      <c r="D73" s="8"/>
-      <c r="E73" s="9" t="s">
+      <c r="D73" s="87"/>
+      <c r="E73" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F73" s="7" t="s">
+      <c r="F73" s="86" t="s">
         <v>39</v>
       </c>
-      <c r="G73" s="10"/>
+      <c r="G73" s="88"/>
     </row>
     <row r="74" spans="1:7" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="B74" s="11" t="s">
+      <c r="B74" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C74" s="12"/>
-      <c r="D74" s="13"/>
-      <c r="E74" s="14" t="s">
+      <c r="C74" s="73"/>
+      <c r="D74" s="74"/>
+      <c r="E74" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F74" s="15" t="s">
+      <c r="F74" s="89" t="s">
         <v>40</v>
       </c>
-      <c r="G74" s="16"/>
+      <c r="G74" s="75"/>
     </row>
     <row r="75" spans="1:7" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="B75" s="11" t="s">
+      <c r="B75" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C75" s="12"/>
-      <c r="D75" s="13"/>
-      <c r="E75" s="14" t="s">
+      <c r="C75" s="73"/>
+      <c r="D75" s="74"/>
+      <c r="E75" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F75" s="12"/>
-      <c r="G75" s="16"/>
+      <c r="F75" s="73"/>
+      <c r="G75" s="75"/>
     </row>
     <row r="76" spans="1:7" ht="24" x14ac:dyDescent="0.25">
-      <c r="B76" s="11" t="s">
+      <c r="B76" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C76" s="12" t="s">
+      <c r="C76" s="73" t="s">
         <v>93</v>
       </c>
-      <c r="D76" s="13"/>
-      <c r="E76" s="14"/>
-      <c r="F76" s="12"/>
-      <c r="G76" s="16"/>
+      <c r="D76" s="74"/>
+      <c r="E76" s="10"/>
+      <c r="F76" s="73"/>
+      <c r="G76" s="75"/>
     </row>
     <row r="77" spans="1:7" ht="24" x14ac:dyDescent="0.25">
-      <c r="B77" s="11" t="s">
+      <c r="B77" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C77" s="12" t="s">
+      <c r="C77" s="73" t="s">
         <v>94</v>
       </c>
-      <c r="D77" s="13"/>
-      <c r="E77" s="17"/>
-      <c r="F77" s="12"/>
-      <c r="G77" s="16"/>
+      <c r="D77" s="74"/>
+      <c r="E77" s="11"/>
+      <c r="F77" s="73"/>
+      <c r="G77" s="75"/>
     </row>
     <row r="78" spans="1:7" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="B78" s="18" t="s">
+      <c r="B78" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="C78" s="19"/>
-      <c r="D78" s="19"/>
-      <c r="E78" s="19"/>
-      <c r="F78" s="19"/>
-      <c r="G78" s="20"/>
+      <c r="C78" s="77"/>
+      <c r="D78" s="77"/>
+      <c r="E78" s="77"/>
+      <c r="F78" s="77"/>
+      <c r="G78" s="78"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B79" s="21"/>
-      <c r="C79" s="22"/>
-      <c r="D79" s="22"/>
-      <c r="E79" s="22"/>
-      <c r="F79" s="22"/>
-      <c r="G79" s="23"/>
+      <c r="B79" s="79"/>
+      <c r="C79" s="80"/>
+      <c r="D79" s="80"/>
+      <c r="E79" s="80"/>
+      <c r="F79" s="80"/>
+      <c r="G79" s="81"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B80" s="24"/>
-      <c r="C80" s="22"/>
-      <c r="D80" s="22"/>
-      <c r="E80" s="22"/>
-      <c r="F80" s="22"/>
-      <c r="G80" s="23"/>
+      <c r="B80" s="82"/>
+      <c r="C80" s="80"/>
+      <c r="D80" s="80"/>
+      <c r="E80" s="80"/>
+      <c r="F80" s="80"/>
+      <c r="G80" s="81"/>
     </row>
     <row r="81" spans="1:14" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B81" s="25"/>
-      <c r="C81" s="26"/>
-      <c r="D81" s="26"/>
-      <c r="E81" s="26"/>
-      <c r="F81" s="26"/>
-      <c r="G81" s="27"/>
+      <c r="B81" s="83"/>
+      <c r="C81" s="84"/>
+      <c r="D81" s="84"/>
+      <c r="E81" s="84"/>
+      <c r="F81" s="84"/>
+      <c r="G81" s="85"/>
     </row>
     <row r="83" spans="1:14" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
@@ -2554,76 +2806,76 @@
       </c>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A84" s="28" t="s">
+      <c r="A84" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B84" s="29" t="s">
+      <c r="B84" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C84" s="29" t="s">
+      <c r="C84" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D84" s="29" t="s">
+      <c r="D84" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E84" s="30" t="s">
+      <c r="E84" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F84" s="29" t="s">
+      <c r="F84" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G84" s="31" t="s">
+      <c r="G84" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I84" s="83" t="s">
+      <c r="I84" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="J84" s="32" t="s">
+      <c r="J84" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="K84" s="32" t="s">
+      <c r="K84" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="L84" s="33" t="s">
+      <c r="L84" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="M84" s="33" t="s">
+      <c r="M84" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="N84" s="32" t="s">
+      <c r="N84" s="16" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A85" s="85">
+      <c r="A85" s="60">
         <v>1</v>
       </c>
-      <c r="B85" s="87" t="s">
+      <c r="B85" s="62" t="s">
         <v>95</v>
       </c>
-      <c r="C85" s="87" t="s">
+      <c r="C85" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="D85" s="87" t="s">
+      <c r="D85" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="E85" s="86" t="s">
+      <c r="E85" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="F85" s="87"/>
-      <c r="G85" s="39" t="s">
+      <c r="F85" s="62"/>
+      <c r="G85" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="I85" s="84">
+      <c r="I85" s="59">
         <v>1</v>
       </c>
       <c r="J85" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="K85" s="82">
+      <c r="K85" s="57">
         <v>1415962923</v>
       </c>
-      <c r="L85" s="82">
+      <c r="L85" s="57">
         <v>1415962923</v>
       </c>
       <c r="M85" s="5">
@@ -2634,7 +2886,7 @@
       </c>
     </row>
     <row r="86" spans="1:14" ht="24" x14ac:dyDescent="0.25">
-      <c r="A86" s="34">
+      <c r="A86" s="18">
         <v>2</v>
       </c>
       <c r="B86" s="4" t="s">
@@ -2646,21 +2898,21 @@
       <c r="D86" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E86" s="84" t="s">
+      <c r="E86" s="59" t="s">
         <v>21</v>
       </c>
       <c r="F86" s="4"/>
       <c r="G86" s="4"/>
-      <c r="I86" s="84">
+      <c r="I86" s="59">
         <v>2</v>
       </c>
       <c r="J86" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="K86" s="82">
+      <c r="K86" s="57">
         <v>1415962923</v>
       </c>
-      <c r="L86" s="82">
+      <c r="L86" s="57">
         <v>1415962923</v>
       </c>
       <c r="M86" s="5">
@@ -2671,80 +2923,80 @@
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A87" s="85">
+      <c r="A87" s="60">
         <v>3</v>
       </c>
-      <c r="B87" s="42" t="s">
+      <c r="B87" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="C87" s="44" t="s">
+      <c r="C87" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="D87" s="44" t="s">
+      <c r="D87" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="E87" s="45" t="s">
+      <c r="E87" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="F87" s="46"/>
-      <c r="G87" s="47"/>
+      <c r="F87" s="30"/>
+      <c r="G87" s="31"/>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A88" s="34">
+      <c r="A88" s="18">
         <v>4</v>
       </c>
-      <c r="B88" s="42" t="s">
+      <c r="B88" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="C88" s="44" t="s">
+      <c r="C88" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="D88" s="44" t="s">
+      <c r="D88" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="E88" s="45" t="s">
+      <c r="E88" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="F88" s="46"/>
-      <c r="G88" s="47"/>
+      <c r="F88" s="30"/>
+      <c r="G88" s="31"/>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A89" s="85">
+      <c r="A89" s="60">
         <v>5</v>
       </c>
-      <c r="B89" s="42" t="s">
+      <c r="B89" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="C89" s="44" t="s">
+      <c r="C89" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="D89" s="44" t="s">
+      <c r="D89" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="E89" s="45" t="s">
+      <c r="E89" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="F89" s="46"/>
-      <c r="G89" s="47"/>
+      <c r="F89" s="30"/>
+      <c r="G89" s="31"/>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A90" s="34">
+      <c r="A90" s="18">
         <v>6</v>
       </c>
-      <c r="B90" s="42" t="s">
+      <c r="B90" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="C90" s="44" t="s">
+      <c r="C90" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="D90" s="44" t="s">
+      <c r="D90" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="E90" s="45" t="s">
+      <c r="E90" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="F90" s="46"/>
-      <c r="G90" s="47"/>
+      <c r="F90" s="30"/>
+      <c r="G90" s="31"/>
     </row>
     <row r="92" spans="1:14" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
@@ -2752,55 +3004,55 @@
       </c>
     </row>
     <row r="93" spans="1:14" ht="24" x14ac:dyDescent="0.25">
-      <c r="A93" s="55" t="s">
+      <c r="A93" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="B93" s="56" t="s">
+      <c r="B93" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="C93" s="57" t="s">
+      <c r="C93" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="D93" s="58"/>
-      <c r="E93" s="56" t="s">
+      <c r="D93" s="65"/>
+      <c r="E93" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="F93" s="56" t="s">
+      <c r="F93" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="G93" s="59" t="s">
+      <c r="G93" s="41" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="94" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A94" s="60">
+      <c r="A94" s="42">
         <v>1</v>
       </c>
-      <c r="B94" s="61" t="s">
+      <c r="B94" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="C94" s="62" t="s">
+      <c r="C94" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="D94" s="63"/>
-      <c r="E94" s="64" t="s">
+      <c r="D94" s="67"/>
+      <c r="E94" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="F94" s="64" t="s">
+      <c r="F94" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="G94" s="65"/>
+      <c r="G94" s="45"/>
     </row>
     <row r="95" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="66">
+      <c r="A95" s="46">
         <v>2</v>
       </c>
-      <c r="B95" s="51"/>
-      <c r="C95" s="67"/>
-      <c r="D95" s="68"/>
-      <c r="E95" s="69"/>
-      <c r="F95" s="69"/>
-      <c r="G95" s="70"/>
+      <c r="B95" s="35"/>
+      <c r="C95" s="68"/>
+      <c r="D95" s="69"/>
+      <c r="E95" s="47"/>
+      <c r="F95" s="47"/>
+      <c r="G95" s="48"/>
     </row>
     <row r="97" spans="1:7" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
@@ -2808,21 +3060,21 @@
       </c>
     </row>
     <row r="98" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="74" t="s">
+      <c r="A98" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="B98" s="75" t="s">
+      <c r="B98" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="C98" s="76" t="s">
+      <c r="C98" s="70" t="s">
         <v>27</v>
       </c>
-      <c r="D98" s="77"/>
-      <c r="E98" s="76" t="s">
+      <c r="D98" s="71"/>
+      <c r="E98" s="70" t="s">
         <v>33</v>
       </c>
-      <c r="F98" s="78"/>
-      <c r="G98" s="79" t="s">
+      <c r="F98" s="72"/>
+      <c r="G98" s="54" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2860,45 +3112,166 @@
       </c>
     </row>
     <row r="102" spans="1:7" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="74" t="s">
+      <c r="A102" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="B102" s="75" t="s">
+      <c r="B102" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="C102" s="76" t="s">
+      <c r="C102" s="70" t="s">
         <v>27</v>
       </c>
-      <c r="D102" s="77"/>
-      <c r="E102" s="76" t="s">
+      <c r="D102" s="71"/>
+      <c r="E102" s="70" t="s">
         <v>36</v>
       </c>
-      <c r="F102" s="77"/>
-      <c r="G102" s="79" t="s">
+      <c r="F102" s="71"/>
+      <c r="G102" s="54" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="114" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C114" s="91" t="s">
+        <v>41</v>
+      </c>
+      <c r="F114" s="90" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="115" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C115" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="F115" s="9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="116" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C116" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F116" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="117" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C117" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F117" s="9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="118" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C118" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="F118" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="119" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C119" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="F119" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="120" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C120" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F120" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="121" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C121" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="122" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C122" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="123" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C123" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="126" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D126" s="90" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="127" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D127" s="9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="128" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D128" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="129" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D129" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="130" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D130" s="9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="131" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D131" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="132" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D132" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="133" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D133" s="9" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="57">
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="C98:D98"/>
-    <mergeCell ref="E98:F98"/>
-    <mergeCell ref="C102:D102"/>
-    <mergeCell ref="E102:F102"/>
-    <mergeCell ref="C76:D76"/>
-    <mergeCell ref="F76:G76"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="F77:G77"/>
-    <mergeCell ref="B78:G78"/>
-    <mergeCell ref="B79:G81"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="F74:G74"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="F75:G75"/>
+    <mergeCell ref="B8:G10"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="F41:G41"/>
     <mergeCell ref="C67:D67"/>
     <mergeCell ref="E67:F67"/>
     <mergeCell ref="B42:G42"/>
@@ -2908,40 +3281,31 @@
     <mergeCell ref="C60:D60"/>
     <mergeCell ref="C63:D63"/>
     <mergeCell ref="E63:F63"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G10"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="F74:G74"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="F75:G75"/>
+    <mergeCell ref="C102:D102"/>
+    <mergeCell ref="E102:F102"/>
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="F77:G77"/>
+    <mergeCell ref="B78:G78"/>
+    <mergeCell ref="B79:G81"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="E98:F98"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L14" r:id="rId1"/>
     <hyperlink ref="L15" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Edit file BLOG_TABLE_Design- add lastname, firstname column in users
</commit_message>
<xml_diff>
--- a/doc/BLOG_TABLE_Design.xlsx
+++ b/doc/BLOG_TABLE_Design.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="103">
   <si>
     <t>Table Information</t>
   </si>
@@ -327,6 +327,12 @@
   </si>
   <si>
     <t>id(pk)</t>
+  </si>
+  <si>
+    <t>Last name</t>
+  </si>
+  <si>
+    <t>First name</t>
   </si>
 </sst>
 </file>
@@ -432,7 +438,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="35">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -656,19 +662,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
@@ -893,7 +886,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -988,25 +981,22 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1021,22 +1011,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1048,65 +1038,65 @@
     <xf numFmtId="22" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1190,13 +1180,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>114</xdr:row>
+      <xdr:row>116</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>118</xdr:row>
+      <xdr:row>120</xdr:row>
       <xdr:rowOff>76201</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1237,13 +1227,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>962025</xdr:colOff>
-      <xdr:row>119</xdr:row>
+      <xdr:row>121</xdr:row>
       <xdr:rowOff>133351</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>126</xdr:row>
+      <xdr:row>128</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1284,13 +1274,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>114</xdr:row>
+      <xdr:row>116</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>460344</xdr:colOff>
-      <xdr:row>132</xdr:row>
+      <xdr:row>134</xdr:row>
       <xdr:rowOff>9526</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1328,13 +1318,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>131</xdr:row>
+      <xdr:row>133</xdr:row>
       <xdr:rowOff>114301</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>131</xdr:row>
+      <xdr:row>133</xdr:row>
       <xdr:rowOff>140422</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1372,13 +1362,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>114</xdr:row>
+      <xdr:row>116</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>114</xdr:row>
+      <xdr:row>116</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1681,10 +1671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q133"/>
+  <dimension ref="A1:Q135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="F128" sqref="F128"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -1715,101 +1705,101 @@
       <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="86" t="s">
+      <c r="C2" s="85" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="87"/>
+      <c r="D2" s="86"/>
       <c r="E2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="86" t="s">
+      <c r="F2" s="85" t="s">
         <v>39</v>
       </c>
-      <c r="G2" s="88"/>
+      <c r="G2" s="87"/>
     </row>
     <row r="3" spans="1:17" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="73"/>
-      <c r="D3" s="74"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="73"/>
       <c r="E3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="89" t="s">
+      <c r="F3" s="88" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="75"/>
+      <c r="G3" s="74"/>
     </row>
     <row r="4" spans="1:17" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="73"/>
-      <c r="D4" s="74"/>
+      <c r="C4" s="72"/>
+      <c r="D4" s="73"/>
       <c r="E4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="73"/>
-      <c r="G4" s="75"/>
+      <c r="F4" s="72"/>
+      <c r="G4" s="74"/>
     </row>
     <row r="5" spans="1:17" ht="24" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="73" t="s">
+      <c r="C5" s="72" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="74"/>
+      <c r="D5" s="73"/>
       <c r="E5" s="10"/>
-      <c r="F5" s="73"/>
-      <c r="G5" s="75"/>
+      <c r="F5" s="72"/>
+      <c r="G5" s="74"/>
     </row>
     <row r="6" spans="1:17" ht="24" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="73" t="s">
+      <c r="C6" s="72" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="74"/>
+      <c r="D6" s="73"/>
       <c r="E6" s="11"/>
-      <c r="F6" s="73"/>
-      <c r="G6" s="75"/>
+      <c r="F6" s="72"/>
+      <c r="G6" s="74"/>
     </row>
     <row r="7" spans="1:17" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="B7" s="76" t="s">
+      <c r="B7" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="77"/>
-      <c r="D7" s="77"/>
-      <c r="E7" s="77"/>
-      <c r="F7" s="77"/>
-      <c r="G7" s="78"/>
+      <c r="C7" s="76"/>
+      <c r="D7" s="76"/>
+      <c r="E7" s="76"/>
+      <c r="F7" s="76"/>
+      <c r="G7" s="77"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="79"/>
-      <c r="C8" s="80"/>
-      <c r="D8" s="80"/>
-      <c r="E8" s="80"/>
-      <c r="F8" s="80"/>
-      <c r="G8" s="81"/>
+      <c r="B8" s="78"/>
+      <c r="C8" s="79"/>
+      <c r="D8" s="79"/>
+      <c r="E8" s="79"/>
+      <c r="F8" s="79"/>
+      <c r="G8" s="80"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="82"/>
-      <c r="C9" s="80"/>
-      <c r="D9" s="80"/>
-      <c r="E9" s="80"/>
-      <c r="F9" s="80"/>
-      <c r="G9" s="81"/>
+      <c r="B9" s="81"/>
+      <c r="C9" s="79"/>
+      <c r="D9" s="79"/>
+      <c r="E9" s="79"/>
+      <c r="F9" s="79"/>
+      <c r="G9" s="80"/>
     </row>
     <row r="10" spans="1:17" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="83"/>
-      <c r="C10" s="84"/>
-      <c r="D10" s="84"/>
-      <c r="E10" s="84"/>
-      <c r="F10" s="84"/>
-      <c r="G10" s="85"/>
+      <c r="B10" s="82"/>
+      <c r="C10" s="83"/>
+      <c r="D10" s="83"/>
+      <c r="E10" s="83"/>
+      <c r="F10" s="83"/>
+      <c r="G10" s="84"/>
     </row>
     <row r="12" spans="1:17" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
@@ -1841,7 +1831,7 @@
       <c r="G13" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I13" s="58" t="s">
+      <c r="I13" s="57" t="s">
         <v>18</v>
       </c>
       <c r="J13" s="16" t="s">
@@ -1889,16 +1879,16 @@
       <c r="G14" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="I14" s="59">
+      <c r="I14" s="58">
         <v>1</v>
       </c>
       <c r="J14" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="K14" s="55" t="s">
+      <c r="K14" s="54" t="s">
         <v>63</v>
       </c>
-      <c r="L14" s="56" t="s">
+      <c r="L14" s="55" t="s">
         <v>64</v>
       </c>
       <c r="M14" s="5" t="s">
@@ -1907,7 +1897,7 @@
       <c r="N14" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="O14" s="57">
+      <c r="O14" s="56">
         <v>1415962923</v>
       </c>
       <c r="P14" s="4" t="s">
@@ -1935,7 +1925,7 @@
       </c>
       <c r="F15" s="30"/>
       <c r="G15" s="31"/>
-      <c r="I15" s="59">
+      <c r="I15" s="58">
         <v>2</v>
       </c>
       <c r="J15" s="4" t="s">
@@ -1944,7 +1934,7 @@
       <c r="K15" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="L15" s="56" t="s">
+      <c r="L15" s="55" t="s">
         <v>69</v>
       </c>
       <c r="M15" s="5" t="s">
@@ -1953,7 +1943,7 @@
       <c r="N15" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="O15" s="57">
+      <c r="O15" s="56">
         <v>1415962923</v>
       </c>
       <c r="P15" s="4" t="s">
@@ -1964,8 +1954,7 @@
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="25">
-        <f t="shared" ref="A16:A20" si="0">A15+1</f>
+      <c r="A16" s="18">
         <v>3</v>
       </c>
       <c r="B16" s="26" t="s">
@@ -1984,18 +1973,17 @@
       <c r="G16" s="31"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="25">
-        <f t="shared" si="0"/>
+      <c r="A17" s="18">
         <v>4</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>49</v>
+        <v>101</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D17" s="28" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E17" s="29" t="s">
         <v>21</v>
@@ -2005,17 +1993,16 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="25">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>52</v>
+        <v>102</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="D18" s="28" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="E18" s="29" t="s">
         <v>21</v>
@@ -2024,18 +2011,17 @@
       <c r="G18" s="31"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="25">
-        <f t="shared" si="0"/>
+      <c r="A19" s="18">
         <v>6</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D19" s="28" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E19" s="29" t="s">
         <v>21</v>
@@ -2043,481 +2029,480 @@
       <c r="F19" s="30"/>
       <c r="G19" s="31"/>
     </row>
-    <row r="20" spans="1:15" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="32">
-        <f t="shared" si="0"/>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="25">
         <v>7</v>
       </c>
-      <c r="B20" s="33" t="s">
+      <c r="B20" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" s="30"/>
+      <c r="G20" s="31"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="18">
+        <v>8</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" s="30"/>
+      <c r="G21" s="31"/>
+    </row>
+    <row r="22" spans="1:15" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="18">
+        <v>9</v>
+      </c>
+      <c r="B22" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="C20" s="34" t="s">
+      <c r="C22" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="D20" s="35" t="s">
+      <c r="D22" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="E20" s="36" t="s">
+      <c r="E22" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="37" t="s">
+      <c r="F22" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="G20" s="38" t="s">
+      <c r="G22" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="N20" s="24"/>
-      <c r="O20" s="24"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="N21" s="24"/>
-      <c r="O21" s="24"/>
-    </row>
-    <row r="22" spans="1:15" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
+      <c r="N22" s="24"/>
+      <c r="O22" s="24"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N23" s="24"/>
+      <c r="O23" s="24"/>
+    </row>
+    <row r="24" spans="1:15" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I22" s="49"/>
-      <c r="J22" s="49"/>
-      <c r="K22" s="49"/>
-      <c r="L22" s="49"/>
-      <c r="M22" s="50"/>
-      <c r="N22" s="51"/>
-      <c r="O22" s="51"/>
-    </row>
-    <row r="23" spans="1:15" ht="24" x14ac:dyDescent="0.25">
-      <c r="A23" s="39" t="s">
+      <c r="I24" s="48"/>
+      <c r="J24" s="48"/>
+      <c r="K24" s="48"/>
+      <c r="L24" s="48"/>
+      <c r="M24" s="49"/>
+      <c r="N24" s="50"/>
+      <c r="O24" s="50"/>
+    </row>
+    <row r="25" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+      <c r="A25" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="40" t="s">
+      <c r="B25" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="64" t="s">
+      <c r="C25" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="65"/>
-      <c r="E23" s="40" t="s">
+      <c r="D25" s="64"/>
+      <c r="E25" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="F23" s="40" t="s">
+      <c r="F25" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="G23" s="41" t="s">
+      <c r="G25" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="I23" s="49"/>
-      <c r="J23" s="49"/>
-      <c r="K23" s="49"/>
-      <c r="L23" s="49"/>
-      <c r="M23" s="50"/>
-      <c r="N23" s="51"/>
-      <c r="O23" s="51"/>
-    </row>
-    <row r="24" spans="1:15" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A24" s="42">
+      <c r="I25" s="48"/>
+      <c r="J25" s="48"/>
+      <c r="K25" s="48"/>
+      <c r="L25" s="48"/>
+      <c r="M25" s="49"/>
+      <c r="N25" s="50"/>
+      <c r="O25" s="50"/>
+    </row>
+    <row r="26" spans="1:15" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A26" s="41">
         <v>1</v>
       </c>
-      <c r="B24" s="43" t="s">
+      <c r="B26" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="66" t="s">
+      <c r="C26" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="67"/>
-      <c r="E24" s="44" t="s">
+      <c r="D26" s="66"/>
+      <c r="E26" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="F24" s="44" t="s">
+      <c r="F26" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="G24" s="45"/>
-      <c r="I24" s="49"/>
-      <c r="J24" s="49"/>
-      <c r="K24" s="49"/>
-      <c r="L24" s="49"/>
-      <c r="M24" s="50"/>
-      <c r="N24" s="51"/>
-      <c r="O24" s="51"/>
-    </row>
-    <row r="25" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="46">
+      <c r="G26" s="44"/>
+      <c r="I26" s="48"/>
+      <c r="J26" s="48"/>
+      <c r="K26" s="48"/>
+      <c r="L26" s="48"/>
+      <c r="M26" s="49"/>
+      <c r="N26" s="50"/>
+      <c r="O26" s="50"/>
+    </row>
+    <row r="27" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="45">
         <v>2</v>
       </c>
-      <c r="B25" s="35"/>
-      <c r="C25" s="68"/>
-      <c r="D25" s="69"/>
-      <c r="E25" s="47"/>
-      <c r="F25" s="47"/>
-      <c r="G25" s="48"/>
-      <c r="I25" s="49"/>
-      <c r="J25" s="49"/>
-      <c r="K25" s="49"/>
-      <c r="L25" s="49"/>
-      <c r="M25" s="50"/>
-      <c r="N25" s="51"/>
-      <c r="O25" s="51"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="N26" s="24"/>
-      <c r="O26" s="24"/>
-    </row>
-    <row r="27" spans="1:15" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
+      <c r="B27" s="34"/>
+      <c r="C27" s="67"/>
+      <c r="D27" s="68"/>
+      <c r="E27" s="46"/>
+      <c r="F27" s="46"/>
+      <c r="G27" s="47"/>
+      <c r="I27" s="48"/>
+      <c r="J27" s="48"/>
+      <c r="K27" s="48"/>
+      <c r="L27" s="48"/>
+      <c r="M27" s="49"/>
+      <c r="N27" s="50"/>
+      <c r="O27" s="50"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N28" s="24"/>
+      <c r="O28" s="24"/>
+    </row>
+    <row r="29" spans="1:15" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="N27" s="24"/>
-      <c r="O27" s="24"/>
-    </row>
-    <row r="28" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="52" t="s">
+      <c r="N29" s="24"/>
+      <c r="O29" s="24"/>
+    </row>
+    <row r="30" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="53" t="s">
+      <c r="B30" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="C28" s="70" t="s">
+      <c r="C30" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="D28" s="71"/>
-      <c r="E28" s="70" t="s">
+      <c r="D30" s="70"/>
+      <c r="E30" s="69" t="s">
         <v>33</v>
       </c>
-      <c r="F28" s="72"/>
-      <c r="G28" s="54" t="s">
+      <c r="F30" s="71"/>
+      <c r="G30" s="53" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
+    <row r="32" spans="1:15" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="52" t="s">
+    <row r="33" spans="1:7" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="B31" s="53" t="s">
+      <c r="B33" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="C31" s="70" t="s">
+      <c r="C33" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="D31" s="71"/>
-      <c r="E31" s="70" t="s">
+      <c r="D33" s="70"/>
+      <c r="E33" s="69" t="s">
         <v>36</v>
       </c>
-      <c r="F31" s="72"/>
-      <c r="G31" s="54" t="s">
+      <c r="F33" s="71"/>
+      <c r="G33" s="53" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
+    <row r="38" spans="1:7" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="B37" s="6" t="s">
+    <row r="39" spans="1:7" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="B39" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C37" s="86" t="s">
+      <c r="C39" s="85" t="s">
         <v>38</v>
       </c>
-      <c r="D37" s="87"/>
-      <c r="E37" s="7" t="s">
+      <c r="D39" s="86"/>
+      <c r="E39" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F37" s="86" t="s">
+      <c r="F39" s="85" t="s">
         <v>39</v>
       </c>
-      <c r="G37" s="88"/>
-    </row>
-    <row r="38" spans="1:15" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="B38" s="8" t="s">
+      <c r="G39" s="87"/>
+    </row>
+    <row r="40" spans="1:7" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="B40" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C38" s="73"/>
-      <c r="D38" s="74"/>
-      <c r="E38" s="10" t="s">
+      <c r="C40" s="72"/>
+      <c r="D40" s="73"/>
+      <c r="E40" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F38" s="89" t="s">
+      <c r="F40" s="88" t="s">
         <v>40</v>
       </c>
-      <c r="G38" s="75"/>
-    </row>
-    <row r="39" spans="1:15" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="B39" s="8" t="s">
+      <c r="G40" s="74"/>
+    </row>
+    <row r="41" spans="1:7" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="B41" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C39" s="73"/>
-      <c r="D39" s="74"/>
-      <c r="E39" s="10" t="s">
+      <c r="C41" s="72"/>
+      <c r="D41" s="73"/>
+      <c r="E41" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F39" s="73"/>
-      <c r="G39" s="75"/>
-    </row>
-    <row r="40" spans="1:15" ht="24" x14ac:dyDescent="0.25">
-      <c r="B40" s="8" t="s">
+      <c r="F41" s="72"/>
+      <c r="G41" s="74"/>
+    </row>
+    <row r="42" spans="1:7" ht="24" x14ac:dyDescent="0.25">
+      <c r="B42" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C40" s="73" t="s">
+      <c r="C42" s="72" t="s">
         <v>71</v>
       </c>
-      <c r="D40" s="74"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="73"/>
-      <c r="G40" s="75"/>
-    </row>
-    <row r="41" spans="1:15" ht="24" x14ac:dyDescent="0.25">
-      <c r="B41" s="8" t="s">
+      <c r="D42" s="73"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="72"/>
+      <c r="G42" s="74"/>
+    </row>
+    <row r="43" spans="1:7" ht="24" x14ac:dyDescent="0.25">
+      <c r="B43" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C41" s="73" t="s">
+      <c r="C43" s="72" t="s">
         <v>72</v>
       </c>
-      <c r="D41" s="74"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="73"/>
-      <c r="G41" s="75"/>
-    </row>
-    <row r="42" spans="1:15" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="B42" s="76" t="s">
+      <c r="D43" s="73"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="72"/>
+      <c r="G43" s="74"/>
+    </row>
+    <row r="44" spans="1:7" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="B44" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="C42" s="77"/>
-      <c r="D42" s="77"/>
-      <c r="E42" s="77"/>
-      <c r="F42" s="77"/>
-      <c r="G42" s="78"/>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B43" s="79"/>
-      <c r="C43" s="80"/>
-      <c r="D43" s="80"/>
-      <c r="E43" s="80"/>
-      <c r="F43" s="80"/>
-      <c r="G43" s="81"/>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B44" s="82"/>
-      <c r="C44" s="80"/>
-      <c r="D44" s="80"/>
-      <c r="E44" s="80"/>
-      <c r="F44" s="80"/>
-      <c r="G44" s="81"/>
-    </row>
-    <row r="45" spans="1:15" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="83"/>
-      <c r="C45" s="84"/>
-      <c r="D45" s="84"/>
-      <c r="E45" s="84"/>
-      <c r="F45" s="84"/>
-      <c r="G45" s="85"/>
-    </row>
-    <row r="47" spans="1:15" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
+      <c r="C44" s="76"/>
+      <c r="D44" s="76"/>
+      <c r="E44" s="76"/>
+      <c r="F44" s="76"/>
+      <c r="G44" s="77"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B45" s="78"/>
+      <c r="C45" s="79"/>
+      <c r="D45" s="79"/>
+      <c r="E45" s="79"/>
+      <c r="F45" s="79"/>
+      <c r="G45" s="80"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B46" s="81"/>
+      <c r="C46" s="79"/>
+      <c r="D46" s="79"/>
+      <c r="E46" s="79"/>
+      <c r="F46" s="79"/>
+      <c r="G46" s="80"/>
+    </row>
+    <row r="47" spans="1:7" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="82"/>
+      <c r="C47" s="83"/>
+      <c r="D47" s="83"/>
+      <c r="E47" s="83"/>
+      <c r="F47" s="83"/>
+      <c r="G47" s="84"/>
+    </row>
+    <row r="49" spans="1:15" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I47" s="4" t="s">
+      <c r="I49" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A48" s="12" t="s">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A50" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B48" s="13" t="s">
+      <c r="B50" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C48" s="13" t="s">
+      <c r="C50" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D48" s="13" t="s">
+      <c r="D50" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E48" s="14" t="s">
+      <c r="E50" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F48" s="13" t="s">
+      <c r="F50" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G48" s="15" t="s">
+      <c r="G50" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I48" s="58" t="s">
+      <c r="I50" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="J48" s="16" t="s">
+      <c r="J50" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="K48" s="16" t="s">
+      <c r="K50" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="L48" s="16" t="s">
+      <c r="L50" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="M48" s="17" t="s">
+      <c r="M50" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="N48" s="16" t="s">
+      <c r="N50" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="O48" s="16" t="s">
+      <c r="O50" s="16" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="49" spans="1:15" ht="24" x14ac:dyDescent="0.25">
-      <c r="A49" s="60">
+    <row r="51" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+      <c r="A51" s="59">
         <v>1</v>
       </c>
-      <c r="B49" s="62" t="s">
+      <c r="B51" s="61" t="s">
         <v>74</v>
       </c>
-      <c r="C49" s="62" t="s">
+      <c r="C51" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="D49" s="62" t="s">
+      <c r="D51" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="E49" s="61" t="s">
+      <c r="E51" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F49" s="62"/>
-      <c r="G49" s="23" t="s">
+      <c r="F51" s="61"/>
+      <c r="G51" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="I49" s="59">
+      <c r="I51" s="58">
         <v>1</v>
       </c>
-      <c r="J49" s="4" t="s">
+      <c r="J51" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="K49" s="5" t="s">
+      <c r="K51" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="L49" s="57">
+      <c r="L51" s="56">
         <v>1415962923</v>
       </c>
-      <c r="M49" s="57">
+      <c r="M51" s="56">
         <v>1415962923</v>
       </c>
-      <c r="N49" s="4">
+      <c r="N51" s="4">
         <v>1</v>
       </c>
-      <c r="O49" s="4">
+      <c r="O51" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:15" ht="24" x14ac:dyDescent="0.25">
-      <c r="A50" s="18">
+    <row r="52" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+      <c r="A52" s="18">
         <v>2</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B52" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C52" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D50" s="4" t="s">
+      <c r="D52" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E50" s="59" t="s">
+      <c r="E52" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="F50" s="4"/>
-      <c r="G50" s="4"/>
-      <c r="I50" s="59">
+      <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
+      <c r="I52" s="58">
         <v>2</v>
       </c>
-      <c r="J50" s="4" t="s">
+      <c r="J52" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="K50" s="5" t="s">
+      <c r="K52" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="L50" s="57">
+      <c r="L52" s="56">
         <v>1415962923</v>
       </c>
-      <c r="M50" s="57">
+      <c r="M52" s="56">
         <v>1415962923</v>
       </c>
-      <c r="N50" s="4">
+      <c r="N52" s="4">
         <v>2</v>
       </c>
-      <c r="O50" s="4">
+      <c r="O52" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A51" s="60">
+    <row r="53" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="A53" s="59">
         <v>3</v>
       </c>
-      <c r="B51" s="26" t="s">
+      <c r="B53" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="C51" s="27" t="s">
+      <c r="C53" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="D51" s="28" t="s">
+      <c r="D53" s="28" t="s">
         <v>24</v>
-      </c>
-      <c r="E51" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="F51" s="30"/>
-      <c r="G51" s="31"/>
-      <c r="I51" s="59"/>
-      <c r="L51" s="63"/>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A52" s="18">
-        <v>4</v>
-      </c>
-      <c r="B52" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="C52" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="D52" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="E52" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="F52" s="30"/>
-      <c r="G52" s="31"/>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A53" s="60">
-        <v>5</v>
-      </c>
-      <c r="B53" s="26" t="s">
-        <v>80</v>
-      </c>
-      <c r="C53" s="28" t="s">
-        <v>81</v>
-      </c>
-      <c r="D53" s="28" t="s">
-        <v>20</v>
       </c>
       <c r="E53" s="29" t="s">
         <v>21</v>
       </c>
       <c r="F53" s="30"/>
       <c r="G53" s="31"/>
+      <c r="I53" s="58"/>
+      <c r="L53" s="62"/>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" s="18">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B54" s="26" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C54" s="28" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D54" s="28" t="s">
         <v>20</v>
@@ -2527,448 +2512,448 @@
       </c>
       <c r="F54" s="30"/>
       <c r="G54" s="31"/>
-      <c r="I54" s="19"/>
-      <c r="J54" s="20"/>
-      <c r="K54" s="19"/>
-      <c r="L54" s="21"/>
-      <c r="M54" s="22"/>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A55" s="60">
-        <v>7</v>
+      <c r="A55" s="59">
+        <v>5</v>
       </c>
       <c r="B55" s="26" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C55" s="28" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="D55" s="28" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="E55" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="F55" s="30" t="s">
+      <c r="F55" s="30"/>
+      <c r="G55" s="31"/>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A56" s="18">
+        <v>6</v>
+      </c>
+      <c r="B56" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="C56" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="D56" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="E56" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="F56" s="30"/>
+      <c r="G56" s="31"/>
+      <c r="I56" s="19"/>
+      <c r="J56" s="20"/>
+      <c r="K56" s="19"/>
+      <c r="L56" s="21"/>
+      <c r="M56" s="22"/>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A57" s="59">
+        <v>7</v>
+      </c>
+      <c r="B57" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="C57" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="D57" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="E57" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="F57" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="G55" s="31" t="s">
+      <c r="G57" s="31" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="57" spans="1:15" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="1" t="s">
+    <row r="59" spans="1:15" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="58" spans="1:15" ht="24" x14ac:dyDescent="0.25">
-      <c r="A58" s="39" t="s">
+    <row r="60" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+      <c r="A60" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="B58" s="40" t="s">
+      <c r="B60" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="C58" s="64" t="s">
+      <c r="C60" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="D58" s="65"/>
-      <c r="E58" s="40" t="s">
+      <c r="D60" s="64"/>
+      <c r="E60" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="F58" s="40" t="s">
+      <c r="F60" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="G58" s="41" t="s">
+      <c r="G60" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="I58" s="49"/>
-      <c r="J58" s="49"/>
-      <c r="K58" s="49"/>
-      <c r="L58" s="49"/>
-    </row>
-    <row r="59" spans="1:15" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A59" s="42">
+      <c r="I60" s="48"/>
+      <c r="J60" s="48"/>
+      <c r="K60" s="48"/>
+      <c r="L60" s="48"/>
+    </row>
+    <row r="61" spans="1:15" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A61" s="41">
         <v>1</v>
       </c>
-      <c r="B59" s="43" t="s">
+      <c r="B61" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="C59" s="66" t="s">
+      <c r="C61" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="D59" s="67"/>
-      <c r="E59" s="44" t="s">
+      <c r="D61" s="66"/>
+      <c r="E61" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="F59" s="44" t="s">
+      <c r="F61" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="G59" s="45"/>
-      <c r="I59" s="49"/>
-      <c r="J59" s="49"/>
-      <c r="K59" s="49"/>
-      <c r="L59" s="49"/>
-    </row>
-    <row r="60" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="46">
+      <c r="G61" s="44"/>
+      <c r="I61" s="48"/>
+      <c r="J61" s="48"/>
+      <c r="K61" s="48"/>
+      <c r="L61" s="48"/>
+    </row>
+    <row r="62" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="45">
         <v>2</v>
       </c>
-      <c r="B60" s="35"/>
-      <c r="C60" s="68"/>
-      <c r="D60" s="69"/>
-      <c r="E60" s="47"/>
-      <c r="F60" s="47"/>
-      <c r="G60" s="48"/>
-      <c r="I60" s="49"/>
-      <c r="J60" s="49"/>
-      <c r="K60" s="49"/>
-      <c r="L60" s="49"/>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I61" s="49"/>
-      <c r="J61" s="49"/>
-      <c r="K61" s="49"/>
-      <c r="L61" s="49"/>
-    </row>
-    <row r="62" spans="1:15" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="1" t="s">
+      <c r="B62" s="34"/>
+      <c r="C62" s="67"/>
+      <c r="D62" s="68"/>
+      <c r="E62" s="46"/>
+      <c r="F62" s="46"/>
+      <c r="G62" s="47"/>
+      <c r="I62" s="48"/>
+      <c r="J62" s="48"/>
+      <c r="K62" s="48"/>
+      <c r="L62" s="48"/>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I63" s="48"/>
+      <c r="J63" s="48"/>
+      <c r="K63" s="48"/>
+      <c r="L63" s="48"/>
+    </row>
+    <row r="64" spans="1:15" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="63" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="52" t="s">
+    <row r="65" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="B63" s="53" t="s">
+      <c r="B65" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="C63" s="70" t="s">
+      <c r="C65" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="D63" s="71"/>
-      <c r="E63" s="70" t="s">
+      <c r="D65" s="70"/>
+      <c r="E65" s="69" t="s">
         <v>33</v>
       </c>
-      <c r="F63" s="72"/>
-      <c r="G63" s="54" t="s">
+      <c r="F65" s="71"/>
+      <c r="G65" s="53" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A64" s="4">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="4">
         <v>1</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="C66" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E64" s="2" t="s">
+      <c r="E66" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G64" s="2" t="s">
+      <c r="G66" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="1" t="s">
+    <row r="68" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="52" t="s">
+    <row r="69" spans="1:7" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="B67" s="53" t="s">
+      <c r="B69" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="C67" s="70" t="s">
+      <c r="C69" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="D67" s="71"/>
-      <c r="E67" s="70" t="s">
+      <c r="D69" s="70"/>
+      <c r="E69" s="69" t="s">
         <v>36</v>
       </c>
-      <c r="F67" s="71"/>
-      <c r="G67" s="54" t="s">
+      <c r="F69" s="70"/>
+      <c r="G69" s="53" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="1" t="s">
+    <row r="74" spans="1:7" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="B73" s="6" t="s">
+    <row r="75" spans="1:7" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="B75" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C73" s="86" t="s">
+      <c r="C75" s="85" t="s">
         <v>38</v>
       </c>
-      <c r="D73" s="87"/>
-      <c r="E73" s="7" t="s">
+      <c r="D75" s="86"/>
+      <c r="E75" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F73" s="86" t="s">
+      <c r="F75" s="85" t="s">
         <v>39</v>
       </c>
-      <c r="G73" s="88"/>
-    </row>
-    <row r="74" spans="1:7" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="B74" s="8" t="s">
+      <c r="G75" s="87"/>
+    </row>
+    <row r="76" spans="1:7" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="B76" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C74" s="73"/>
-      <c r="D74" s="74"/>
-      <c r="E74" s="10" t="s">
+      <c r="C76" s="72"/>
+      <c r="D76" s="73"/>
+      <c r="E76" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F74" s="89" t="s">
+      <c r="F76" s="88" t="s">
         <v>40</v>
       </c>
-      <c r="G74" s="75"/>
-    </row>
-    <row r="75" spans="1:7" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="B75" s="8" t="s">
+      <c r="G76" s="74"/>
+    </row>
+    <row r="77" spans="1:7" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="B77" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C75" s="73"/>
-      <c r="D75" s="74"/>
-      <c r="E75" s="10" t="s">
+      <c r="C77" s="72"/>
+      <c r="D77" s="73"/>
+      <c r="E77" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F75" s="73"/>
-      <c r="G75" s="75"/>
-    </row>
-    <row r="76" spans="1:7" ht="24" x14ac:dyDescent="0.25">
-      <c r="B76" s="8" t="s">
+      <c r="F77" s="72"/>
+      <c r="G77" s="74"/>
+    </row>
+    <row r="78" spans="1:7" ht="24" x14ac:dyDescent="0.25">
+      <c r="B78" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C76" s="73" t="s">
+      <c r="C78" s="72" t="s">
         <v>93</v>
       </c>
-      <c r="D76" s="74"/>
-      <c r="E76" s="10"/>
-      <c r="F76" s="73"/>
-      <c r="G76" s="75"/>
-    </row>
-    <row r="77" spans="1:7" ht="24" x14ac:dyDescent="0.25">
-      <c r="B77" s="8" t="s">
+      <c r="D78" s="73"/>
+      <c r="E78" s="10"/>
+      <c r="F78" s="72"/>
+      <c r="G78" s="74"/>
+    </row>
+    <row r="79" spans="1:7" ht="24" x14ac:dyDescent="0.25">
+      <c r="B79" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C77" s="73" t="s">
+      <c r="C79" s="72" t="s">
         <v>94</v>
       </c>
-      <c r="D77" s="74"/>
-      <c r="E77" s="11"/>
-      <c r="F77" s="73"/>
-      <c r="G77" s="75"/>
-    </row>
-    <row r="78" spans="1:7" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="B78" s="76" t="s">
+      <c r="D79" s="73"/>
+      <c r="E79" s="11"/>
+      <c r="F79" s="72"/>
+      <c r="G79" s="74"/>
+    </row>
+    <row r="80" spans="1:7" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="B80" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="C78" s="77"/>
-      <c r="D78" s="77"/>
-      <c r="E78" s="77"/>
-      <c r="F78" s="77"/>
-      <c r="G78" s="78"/>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B79" s="79"/>
-      <c r="C79" s="80"/>
-      <c r="D79" s="80"/>
-      <c r="E79" s="80"/>
-      <c r="F79" s="80"/>
-      <c r="G79" s="81"/>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B80" s="82"/>
-      <c r="C80" s="80"/>
-      <c r="D80" s="80"/>
-      <c r="E80" s="80"/>
-      <c r="F80" s="80"/>
-      <c r="G80" s="81"/>
-    </row>
-    <row r="81" spans="1:14" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B81" s="83"/>
-      <c r="C81" s="84"/>
-      <c r="D81" s="84"/>
-      <c r="E81" s="84"/>
-      <c r="F81" s="84"/>
-      <c r="G81" s="85"/>
+      <c r="C80" s="76"/>
+      <c r="D80" s="76"/>
+      <c r="E80" s="76"/>
+      <c r="F80" s="76"/>
+      <c r="G80" s="77"/>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B81" s="78"/>
+      <c r="C81" s="79"/>
+      <c r="D81" s="79"/>
+      <c r="E81" s="79"/>
+      <c r="F81" s="79"/>
+      <c r="G81" s="80"/>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B82" s="81"/>
+      <c r="C82" s="79"/>
+      <c r="D82" s="79"/>
+      <c r="E82" s="79"/>
+      <c r="F82" s="79"/>
+      <c r="G82" s="80"/>
     </row>
     <row r="83" spans="1:14" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="1" t="s">
+      <c r="B83" s="82"/>
+      <c r="C83" s="83"/>
+      <c r="D83" s="83"/>
+      <c r="E83" s="83"/>
+      <c r="F83" s="83"/>
+      <c r="G83" s="84"/>
+    </row>
+    <row r="85" spans="1:14" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I83" s="4" t="s">
+      <c r="I85" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A84" s="12" t="s">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A86" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B84" s="13" t="s">
+      <c r="B86" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C84" s="13" t="s">
+      <c r="C86" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D84" s="13" t="s">
+      <c r="D86" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E84" s="14" t="s">
+      <c r="E86" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F84" s="13" t="s">
+      <c r="F86" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G84" s="15" t="s">
+      <c r="G86" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I84" s="58" t="s">
+      <c r="I86" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="J84" s="16" t="s">
+      <c r="J86" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="K84" s="16" t="s">
+      <c r="K86" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="L84" s="17" t="s">
+      <c r="L86" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="M84" s="17" t="s">
+      <c r="M86" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="N84" s="16" t="s">
+      <c r="N86" s="16" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A85" s="60">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A87" s="59">
         <v>1</v>
       </c>
-      <c r="B85" s="62" t="s">
+      <c r="B87" s="61" t="s">
         <v>95</v>
       </c>
-      <c r="C85" s="62" t="s">
+      <c r="C87" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="D85" s="62" t="s">
+      <c r="D87" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="E85" s="61" t="s">
+      <c r="E87" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F85" s="62"/>
-      <c r="G85" s="23" t="s">
+      <c r="F87" s="61"/>
+      <c r="G87" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="I85" s="59">
+      <c r="I87" s="58">
         <v>1</v>
       </c>
-      <c r="J85" s="5" t="s">
+      <c r="J87" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="K85" s="57">
+      <c r="K87" s="56">
         <v>1415962923</v>
       </c>
-      <c r="L85" s="57">
+      <c r="L87" s="56">
         <v>1415962923</v>
       </c>
-      <c r="M85" s="5">
+      <c r="M87" s="5">
         <v>1</v>
       </c>
-      <c r="N85" s="4">
+      <c r="N87" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:14" ht="24" x14ac:dyDescent="0.25">
-      <c r="A86" s="18">
+    <row r="88" spans="1:14" ht="24" x14ac:dyDescent="0.25">
+      <c r="A88" s="18">
         <v>2</v>
       </c>
-      <c r="B86" s="4" t="s">
+      <c r="B88" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C86" s="4" t="s">
+      <c r="C88" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D86" s="4" t="s">
+      <c r="D88" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E86" s="59" t="s">
+      <c r="E88" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="F86" s="4"/>
-      <c r="G86" s="4"/>
-      <c r="I86" s="59">
+      <c r="F88" s="4"/>
+      <c r="G88" s="4"/>
+      <c r="I88" s="58">
         <v>2</v>
       </c>
-      <c r="J86" s="5" t="s">
+      <c r="J88" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="K86" s="57">
+      <c r="K88" s="56">
         <v>1415962923</v>
       </c>
-      <c r="L86" s="57">
+      <c r="L88" s="56">
         <v>1415962923</v>
       </c>
-      <c r="M86" s="5">
+      <c r="M88" s="5">
         <v>1</v>
       </c>
-      <c r="N86" s="4">
+      <c r="N88" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A87" s="60">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A89" s="59">
         <v>3</v>
       </c>
-      <c r="B87" s="26" t="s">
+      <c r="B89" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="C87" s="28" t="s">
+      <c r="C89" s="28" t="s">
         <v>79</v>
-      </c>
-      <c r="D87" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="E87" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="F87" s="30"/>
-      <c r="G87" s="31"/>
-    </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A88" s="18">
-        <v>4</v>
-      </c>
-      <c r="B88" s="26" t="s">
-        <v>80</v>
-      </c>
-      <c r="C88" s="28" t="s">
-        <v>81</v>
-      </c>
-      <c r="D88" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="E88" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="F88" s="30"/>
-      <c r="G88" s="31"/>
-    </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A89" s="60">
-        <v>5</v>
-      </c>
-      <c r="B89" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="C89" s="28" t="s">
-        <v>83</v>
       </c>
       <c r="D89" s="28" t="s">
         <v>20</v>
@@ -2981,13 +2966,13 @@
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" s="18">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B90" s="26" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="C90" s="28" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="D90" s="28" t="s">
         <v>20</v>
@@ -2998,246 +2983,284 @@
       <c r="F90" s="30"/>
       <c r="G90" s="31"/>
     </row>
-    <row r="92" spans="1:14" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="1" t="s">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A91" s="59">
+        <v>5</v>
+      </c>
+      <c r="B91" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="C91" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="D91" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="E91" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="F91" s="30"/>
+      <c r="G91" s="31"/>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A92" s="18">
+        <v>6</v>
+      </c>
+      <c r="B92" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="C92" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="D92" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="E92" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="F92" s="30"/>
+      <c r="G92" s="31"/>
+    </row>
+    <row r="94" spans="1:14" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="93" spans="1:14" ht="24" x14ac:dyDescent="0.25">
-      <c r="A93" s="39" t="s">
+    <row r="95" spans="1:14" ht="24" x14ac:dyDescent="0.25">
+      <c r="A95" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="B93" s="40" t="s">
+      <c r="B95" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="C93" s="64" t="s">
+      <c r="C95" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="D93" s="65"/>
-      <c r="E93" s="40" t="s">
+      <c r="D95" s="64"/>
+      <c r="E95" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="F93" s="40" t="s">
+      <c r="F95" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="G93" s="41" t="s">
+      <c r="G95" s="40" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A94" s="42">
+    <row r="96" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A96" s="41">
         <v>1</v>
       </c>
-      <c r="B94" s="43" t="s">
+      <c r="B96" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="C94" s="66" t="s">
+      <c r="C96" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="D94" s="67"/>
-      <c r="E94" s="44" t="s">
+      <c r="D96" s="66"/>
+      <c r="E96" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="F94" s="44" t="s">
+      <c r="F96" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="G94" s="45"/>
-    </row>
-    <row r="95" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="46">
+      <c r="G96" s="44"/>
+    </row>
+    <row r="97" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="45">
         <v>2</v>
       </c>
-      <c r="B95" s="35"/>
-      <c r="C95" s="68"/>
-      <c r="D95" s="69"/>
-      <c r="E95" s="47"/>
-      <c r="F95" s="47"/>
-      <c r="G95" s="48"/>
-    </row>
-    <row r="97" spans="1:7" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="1" t="s">
+      <c r="B97" s="34"/>
+      <c r="C97" s="67"/>
+      <c r="D97" s="68"/>
+      <c r="E97" s="46"/>
+      <c r="F97" s="46"/>
+      <c r="G97" s="47"/>
+    </row>
+    <row r="99" spans="1:7" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="52" t="s">
+    <row r="100" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="B98" s="53" t="s">
+      <c r="B100" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="C98" s="70" t="s">
+      <c r="C100" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="D98" s="71"/>
-      <c r="E98" s="70" t="s">
+      <c r="D100" s="70"/>
+      <c r="E100" s="69" t="s">
         <v>33</v>
       </c>
-      <c r="F98" s="72"/>
-      <c r="G98" s="54" t="s">
+      <c r="F100" s="71"/>
+      <c r="G100" s="53" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A99" s="4">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" s="4">
         <v>1</v>
       </c>
-      <c r="C99" s="2" t="s">
+      <c r="C101" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E99" s="2" t="s">
+      <c r="E101" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G99" s="2" t="s">
+      <c r="G101" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A100" s="4">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" s="4">
         <v>2</v>
       </c>
-      <c r="C100" s="2" t="s">
+      <c r="C102" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E100" s="2" t="s">
+      <c r="E102" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G100" s="2" t="s">
+      <c r="G102" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="1" t="s">
+    <row r="103" spans="1:7" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="52" t="s">
+    <row r="104" spans="1:7" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="B102" s="53" t="s">
+      <c r="B104" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="C102" s="70" t="s">
+      <c r="C104" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="D102" s="71"/>
-      <c r="E102" s="70" t="s">
+      <c r="D104" s="70"/>
+      <c r="E104" s="69" t="s">
         <v>36</v>
       </c>
-      <c r="F102" s="71"/>
-      <c r="G102" s="54" t="s">
+      <c r="F104" s="70"/>
+      <c r="G104" s="53" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="114" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C114" s="91" t="s">
+    <row r="116" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C116" s="90" t="s">
         <v>41</v>
       </c>
-      <c r="F114" s="90" t="s">
+      <c r="F116" s="89" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="115" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C115" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="F115" s="9" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="116" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C116" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F116" s="9" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="117" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C117" s="9" t="s">
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="F117" s="9" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
     </row>
     <row r="118" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C118" s="9" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="F118" s="9" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="119" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C119" s="9" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="F119" s="9" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="120" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C120" s="9" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F120" s="9" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
     </row>
     <row r="121" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C121" s="9" t="s">
-        <v>53</v>
+        <v>60</v>
+      </c>
+      <c r="F121" s="9" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="122" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C122" s="9" t="s">
-        <v>55</v>
+        <v>61</v>
+      </c>
+      <c r="F122" s="9" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="123" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C123" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="124" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C124" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="125" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C125" s="9" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="126" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D126" s="90" t="s">
+    <row r="128" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D128" s="89" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="127" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D127" s="9" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="128" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D128" s="9" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="129" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D129" s="9" t="s">
-        <v>77</v>
+        <v>100</v>
       </c>
     </row>
     <row r="130" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D130" s="9" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="131" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D131" s="9" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="132" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D132" s="9" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="133" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D133" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="134" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D134" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="135" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D135" s="9" t="s">
         <v>57</v>
       </c>
     </row>
@@ -3255,51 +3278,51 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="B7:G7"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
     <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="E30:F30"/>
     <mergeCell ref="C39:D39"/>
     <mergeCell ref="F39:G39"/>
     <mergeCell ref="C40:D40"/>
     <mergeCell ref="F40:G40"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E33:F33"/>
     <mergeCell ref="C41:D41"/>
     <mergeCell ref="F41:G41"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="E67:F67"/>
-    <mergeCell ref="B42:G42"/>
-    <mergeCell ref="B43:G45"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="E69:F69"/>
+    <mergeCell ref="B44:G44"/>
+    <mergeCell ref="B45:G47"/>
     <mergeCell ref="C60:D60"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="E63:F63"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="F74:G74"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="E65:F65"/>
     <mergeCell ref="C75:D75"/>
     <mergeCell ref="F75:G75"/>
-    <mergeCell ref="C102:D102"/>
-    <mergeCell ref="E102:F102"/>
     <mergeCell ref="C76:D76"/>
     <mergeCell ref="F76:G76"/>
     <mergeCell ref="C77:D77"/>
     <mergeCell ref="F77:G77"/>
-    <mergeCell ref="B78:G78"/>
-    <mergeCell ref="B79:G81"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="C104:D104"/>
+    <mergeCell ref="E104:F104"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="F78:G78"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="F79:G79"/>
+    <mergeCell ref="B80:G80"/>
+    <mergeCell ref="B81:G83"/>
     <mergeCell ref="C95:D95"/>
-    <mergeCell ref="C98:D98"/>
-    <mergeCell ref="E98:F98"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="C100:D100"/>
+    <mergeCell ref="E100:F100"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L14" r:id="rId1"/>

</xml_diff>

<commit_message>
add create_at , modified_at into tables users
</commit_message>
<xml_diff>
--- a/doc/BLOG_TABLE_Design.xlsx
+++ b/doc/BLOG_TABLE_Design.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="103">
   <si>
     <t>Table Information</t>
   </si>
@@ -1180,13 +1180,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>116</xdr:row>
+      <xdr:row>118</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>120</xdr:row>
+      <xdr:row>122</xdr:row>
       <xdr:rowOff>76201</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1227,13 +1227,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>962025</xdr:colOff>
-      <xdr:row>121</xdr:row>
+      <xdr:row>123</xdr:row>
       <xdr:rowOff>133351</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>128</xdr:row>
+      <xdr:row>130</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1274,13 +1274,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>116</xdr:row>
+      <xdr:row>118</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>460344</xdr:colOff>
-      <xdr:row>134</xdr:row>
+      <xdr:row>136</xdr:row>
       <xdr:rowOff>9526</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1318,13 +1318,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>133</xdr:row>
+      <xdr:row>135</xdr:row>
       <xdr:rowOff>114301</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>133</xdr:row>
+      <xdr:row>135</xdr:row>
       <xdr:rowOff>140422</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1362,13 +1362,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>116</xdr:row>
+      <xdr:row>118</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>116</xdr:row>
+      <xdr:row>118</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1671,10 +1671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q135"/>
+  <dimension ref="A1:S137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -1690,18 +1690,19 @@
     <col min="11" max="11" width="24" style="4" customWidth="1"/>
     <col min="12" max="12" width="15.42578125" style="4" customWidth="1"/>
     <col min="13" max="13" width="13" style="5" customWidth="1"/>
-    <col min="14" max="14" width="9.28515625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="15" style="4" customWidth="1"/>
     <col min="15" max="15" width="12.7109375" style="4" customWidth="1"/>
-    <col min="16" max="16" width="14.85546875" style="4" customWidth="1"/>
-    <col min="17" max="16384" width="8.85546875" style="4"/>
+    <col min="16" max="16" width="9.140625" style="4" customWidth="1"/>
+    <col min="17" max="17" width="11.140625" style="4" customWidth="1"/>
+    <col min="18" max="16384" width="8.85546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
@@ -1717,7 +1718,7 @@
       </c>
       <c r="G2" s="87"/>
     </row>
-    <row r="3" spans="1:17" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
         <v>3</v>
       </c>
@@ -1731,7 +1732,7 @@
       </c>
       <c r="G3" s="74"/>
     </row>
-    <row r="4" spans="1:17" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
         <v>5</v>
       </c>
@@ -1743,7 +1744,7 @@
       <c r="F4" s="72"/>
       <c r="G4" s="74"/>
     </row>
-    <row r="5" spans="1:17" ht="24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="24" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
         <v>7</v>
       </c>
@@ -1755,7 +1756,7 @@
       <c r="F5" s="72"/>
       <c r="G5" s="74"/>
     </row>
-    <row r="6" spans="1:17" ht="24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="24" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>8</v>
       </c>
@@ -1767,7 +1768,7 @@
       <c r="F6" s="72"/>
       <c r="G6" s="74"/>
     </row>
-    <row r="7" spans="1:17" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B7" s="75" t="s">
         <v>9</v>
       </c>
@@ -1777,7 +1778,7 @@
       <c r="F7" s="76"/>
       <c r="G7" s="77"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B8" s="78"/>
       <c r="C8" s="79"/>
       <c r="D8" s="79"/>
@@ -1785,7 +1786,7 @@
       <c r="F8" s="79"/>
       <c r="G8" s="80"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B9" s="81"/>
       <c r="C9" s="79"/>
       <c r="D9" s="79"/>
@@ -1793,7 +1794,7 @@
       <c r="F9" s="79"/>
       <c r="G9" s="80"/>
     </row>
-    <row r="10" spans="1:17" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="82"/>
       <c r="C10" s="83"/>
       <c r="D10" s="83"/>
@@ -1801,7 +1802,7 @@
       <c r="F10" s="83"/>
       <c r="G10" s="84"/>
     </row>
-    <row r="12" spans="1:17" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1809,7 +1810,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>12</v>
       </c>
@@ -1844,22 +1845,28 @@
         <v>50</v>
       </c>
       <c r="M13" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="N13" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="O13" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="N13" s="16" t="s">
+      <c r="P13" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="O13" s="16" t="s">
+      <c r="Q13" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="P13" s="16" t="s">
+      <c r="R13" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="Q13" s="16" t="s">
+      <c r="S13" s="16" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="18">
         <v>1</v>
       </c>
@@ -1891,23 +1898,29 @@
       <c r="L14" s="55" t="s">
         <v>64</v>
       </c>
-      <c r="M14" s="5" t="s">
+      <c r="M14" s="56">
+        <v>1415962923</v>
+      </c>
+      <c r="N14" s="56">
+        <v>1415962923</v>
+      </c>
+      <c r="O14" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="N14" s="24" t="s">
+      <c r="P14" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="O14" s="56">
+      <c r="Q14" s="56">
         <v>1415962923</v>
       </c>
-      <c r="P14" s="4" t="s">
+      <c r="R14" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="Q14" s="4">
+      <c r="S14" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="25">
         <v>2</v>
       </c>
@@ -1937,23 +1950,29 @@
       <c r="L15" s="55" t="s">
         <v>69</v>
       </c>
-      <c r="M15" s="5" t="s">
+      <c r="M15" s="56">
+        <v>1415962923</v>
+      </c>
+      <c r="N15" s="56">
+        <v>1415962923</v>
+      </c>
+      <c r="O15" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="N15" s="24" t="s">
+      <c r="P15" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="O15" s="56">
+      <c r="Q15" s="56">
         <v>1415962923</v>
       </c>
-      <c r="P15" s="4" t="s">
+      <c r="R15" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="Q15" s="4">
+      <c r="S15" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="18">
         <v>3</v>
       </c>
@@ -2034,10 +2053,10 @@
         <v>7</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="C20" s="28" t="s">
-        <v>53</v>
+        <v>79</v>
       </c>
       <c r="D20" s="28" t="s">
         <v>20</v>
@@ -2052,108 +2071,92 @@
       <c r="A21" s="18">
         <v>8</v>
       </c>
-      <c r="B21" s="26" t="s">
+      <c r="B21" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" s="58" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="25">
+        <v>9</v>
+      </c>
+      <c r="B22" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" s="30"/>
+      <c r="G22" s="31"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="18">
+        <v>10</v>
+      </c>
+      <c r="B23" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="C21" s="28" t="s">
+      <c r="C23" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="D21" s="28" t="s">
+      <c r="D23" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="E21" s="29" t="s">
+      <c r="E23" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="30"/>
-      <c r="G21" s="31"/>
-    </row>
-    <row r="22" spans="1:15" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="18">
-        <v>9</v>
-      </c>
-      <c r="B22" s="32" t="s">
+      <c r="F23" s="30"/>
+      <c r="G23" s="31"/>
+    </row>
+    <row r="24" spans="1:15" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="18">
+        <v>11</v>
+      </c>
+      <c r="B24" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="C22" s="33" t="s">
+      <c r="C24" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="D22" s="34" t="s">
+      <c r="D24" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="E22" s="35" t="s">
+      <c r="E24" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="F22" s="36" t="s">
+      <c r="F24" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="G22" s="37" t="s">
+      <c r="G24" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="N22" s="24"/>
-      <c r="O22" s="24"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="N23" s="24"/>
-      <c r="O23" s="24"/>
-    </row>
-    <row r="24" spans="1:15" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
+      <c r="N24" s="24"/>
+      <c r="O24" s="24"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N25" s="24"/>
+      <c r="O25" s="24"/>
+    </row>
+    <row r="26" spans="1:15" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I24" s="48"/>
-      <c r="J24" s="48"/>
-      <c r="K24" s="48"/>
-      <c r="L24" s="48"/>
-      <c r="M24" s="49"/>
-      <c r="N24" s="50"/>
-      <c r="O24" s="50"/>
-    </row>
-    <row r="25" spans="1:15" ht="24" x14ac:dyDescent="0.25">
-      <c r="A25" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="63" t="s">
-        <v>27</v>
-      </c>
-      <c r="D25" s="64"/>
-      <c r="E25" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="F25" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="G25" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="I25" s="48"/>
-      <c r="J25" s="48"/>
-      <c r="K25" s="48"/>
-      <c r="L25" s="48"/>
-      <c r="M25" s="49"/>
-      <c r="N25" s="50"/>
-      <c r="O25" s="50"/>
-    </row>
-    <row r="26" spans="1:15" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A26" s="41">
-        <v>1</v>
-      </c>
-      <c r="B26" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="C26" s="65" t="s">
-        <v>18</v>
-      </c>
-      <c r="D26" s="66"/>
-      <c r="E26" s="43" t="s">
-        <v>21</v>
-      </c>
-      <c r="F26" s="43" t="s">
-        <v>21</v>
-      </c>
-      <c r="G26" s="44"/>
       <c r="I26" s="48"/>
       <c r="J26" s="48"/>
       <c r="K26" s="48"/>
@@ -2162,16 +2165,26 @@
       <c r="N26" s="50"/>
       <c r="O26" s="50"/>
     </row>
-    <row r="27" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="45">
-        <v>2</v>
-      </c>
-      <c r="B27" s="34"/>
-      <c r="C27" s="67"/>
-      <c r="D27" s="68"/>
-      <c r="E27" s="46"/>
-      <c r="F27" s="46"/>
-      <c r="G27" s="47"/>
+    <row r="27" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+      <c r="A27" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="63" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" s="64"/>
+      <c r="E27" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="F27" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="G27" s="40" t="s">
+        <v>9</v>
+      </c>
       <c r="I27" s="48"/>
       <c r="J27" s="48"/>
       <c r="K27" s="48"/>
@@ -2180,367 +2193,384 @@
       <c r="N27" s="50"/>
       <c r="O27" s="50"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="N28" s="24"/>
-      <c r="O28" s="24"/>
-    </row>
-    <row r="29" spans="1:15" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
+    <row r="28" spans="1:15" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A28" s="41">
+        <v>1</v>
+      </c>
+      <c r="B28" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" s="65" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" s="66"/>
+      <c r="E28" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="F28" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="G28" s="44"/>
+      <c r="I28" s="48"/>
+      <c r="J28" s="48"/>
+      <c r="K28" s="48"/>
+      <c r="L28" s="48"/>
+      <c r="M28" s="49"/>
+      <c r="N28" s="50"/>
+      <c r="O28" s="50"/>
+    </row>
+    <row r="29" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="45">
+        <v>2</v>
+      </c>
+      <c r="B29" s="34"/>
+      <c r="C29" s="67"/>
+      <c r="D29" s="68"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="47"/>
+      <c r="I29" s="48"/>
+      <c r="J29" s="48"/>
+      <c r="K29" s="48"/>
+      <c r="L29" s="48"/>
+      <c r="M29" s="49"/>
+      <c r="N29" s="50"/>
+      <c r="O29" s="50"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N30" s="24"/>
+      <c r="O30" s="24"/>
+    </row>
+    <row r="31" spans="1:15" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="N29" s="24"/>
-      <c r="O29" s="24"/>
-    </row>
-    <row r="30" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="51" t="s">
+      <c r="N31" s="24"/>
+      <c r="O31" s="24"/>
+    </row>
+    <row r="32" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="B30" s="52" t="s">
+      <c r="B32" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="C30" s="69" t="s">
+      <c r="C32" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="D30" s="70"/>
-      <c r="E30" s="69" t="s">
+      <c r="D32" s="70"/>
+      <c r="E32" s="69" t="s">
         <v>33</v>
       </c>
-      <c r="F30" s="71"/>
-      <c r="G30" s="53" t="s">
+      <c r="F32" s="71"/>
+      <c r="G32" s="53" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
+    <row r="34" spans="1:13" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="51" t="s">
+    <row r="35" spans="1:13" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="B33" s="52" t="s">
+      <c r="B35" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="C33" s="69" t="s">
+      <c r="C35" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="D33" s="70"/>
-      <c r="E33" s="69" t="s">
+      <c r="D35" s="70"/>
+      <c r="E35" s="69" t="s">
         <v>36</v>
       </c>
-      <c r="F33" s="71"/>
-      <c r="G33" s="53" t="s">
+      <c r="F35" s="71"/>
+      <c r="G35" s="53" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
+      <c r="M35" s="4"/>
+    </row>
+    <row r="40" spans="1:13" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="B39" s="6" t="s">
+      <c r="M40" s="4"/>
+    </row>
+    <row r="41" spans="1:13" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="B41" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C39" s="85" t="s">
+      <c r="C41" s="85" t="s">
         <v>38</v>
       </c>
-      <c r="D39" s="86"/>
-      <c r="E39" s="7" t="s">
+      <c r="D41" s="86"/>
+      <c r="E41" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F39" s="85" t="s">
+      <c r="F41" s="85" t="s">
         <v>39</v>
       </c>
-      <c r="G39" s="87"/>
-    </row>
-    <row r="40" spans="1:7" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="B40" s="8" t="s">
+      <c r="G41" s="87"/>
+      <c r="M41" s="4"/>
+    </row>
+    <row r="42" spans="1:13" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="B42" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C40" s="72"/>
-      <c r="D40" s="73"/>
-      <c r="E40" s="10" t="s">
+      <c r="C42" s="72"/>
+      <c r="D42" s="73"/>
+      <c r="E42" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F40" s="88" t="s">
+      <c r="F42" s="88" t="s">
         <v>40</v>
       </c>
-      <c r="G40" s="74"/>
-    </row>
-    <row r="41" spans="1:7" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="B41" s="8" t="s">
+      <c r="G42" s="74"/>
+      <c r="M42" s="4"/>
+    </row>
+    <row r="43" spans="1:13" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="B43" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C41" s="72"/>
-      <c r="D41" s="73"/>
-      <c r="E41" s="10" t="s">
+      <c r="C43" s="72"/>
+      <c r="D43" s="73"/>
+      <c r="E43" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F41" s="72"/>
-      <c r="G41" s="74"/>
-    </row>
-    <row r="42" spans="1:7" ht="24" x14ac:dyDescent="0.25">
-      <c r="B42" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C42" s="72" t="s">
-        <v>71</v>
-      </c>
-      <c r="D42" s="73"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="72"/>
-      <c r="G42" s="74"/>
-    </row>
-    <row r="43" spans="1:7" ht="24" x14ac:dyDescent="0.25">
-      <c r="B43" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C43" s="72" t="s">
-        <v>72</v>
-      </c>
-      <c r="D43" s="73"/>
-      <c r="E43" s="11"/>
       <c r="F43" s="72"/>
       <c r="G43" s="74"/>
-    </row>
-    <row r="44" spans="1:7" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="B44" s="75" t="s">
+      <c r="M43" s="4"/>
+    </row>
+    <row r="44" spans="1:13" ht="24" x14ac:dyDescent="0.25">
+      <c r="B44" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" s="72" t="s">
+        <v>71</v>
+      </c>
+      <c r="D44" s="73"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="72"/>
+      <c r="G44" s="74"/>
+      <c r="M44" s="4"/>
+    </row>
+    <row r="45" spans="1:13" ht="24" x14ac:dyDescent="0.25">
+      <c r="B45" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" s="72" t="s">
+        <v>72</v>
+      </c>
+      <c r="D45" s="73"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="72"/>
+      <c r="G45" s="74"/>
+      <c r="M45" s="4"/>
+    </row>
+    <row r="46" spans="1:13" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="B46" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="C44" s="76"/>
-      <c r="D44" s="76"/>
-      <c r="E44" s="76"/>
-      <c r="F44" s="76"/>
-      <c r="G44" s="77"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B45" s="78"/>
-      <c r="C45" s="79"/>
-      <c r="D45" s="79"/>
-      <c r="E45" s="79"/>
-      <c r="F45" s="79"/>
-      <c r="G45" s="80"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B46" s="81"/>
-      <c r="C46" s="79"/>
-      <c r="D46" s="79"/>
-      <c r="E46" s="79"/>
-      <c r="F46" s="79"/>
-      <c r="G46" s="80"/>
-    </row>
-    <row r="47" spans="1:7" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="82"/>
-      <c r="C47" s="83"/>
-      <c r="D47" s="83"/>
-      <c r="E47" s="83"/>
-      <c r="F47" s="83"/>
-      <c r="G47" s="84"/>
+      <c r="C46" s="76"/>
+      <c r="D46" s="76"/>
+      <c r="E46" s="76"/>
+      <c r="F46" s="76"/>
+      <c r="G46" s="77"/>
+      <c r="M46" s="4"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B47" s="78"/>
+      <c r="C47" s="79"/>
+      <c r="D47" s="79"/>
+      <c r="E47" s="79"/>
+      <c r="F47" s="79"/>
+      <c r="G47" s="80"/>
+      <c r="M47" s="4"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B48" s="81"/>
+      <c r="C48" s="79"/>
+      <c r="D48" s="79"/>
+      <c r="E48" s="79"/>
+      <c r="F48" s="79"/>
+      <c r="G48" s="80"/>
+      <c r="M48" s="4"/>
     </row>
     <row r="49" spans="1:15" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
+      <c r="B49" s="82"/>
+      <c r="C49" s="83"/>
+      <c r="D49" s="83"/>
+      <c r="E49" s="83"/>
+      <c r="F49" s="83"/>
+      <c r="G49" s="84"/>
+      <c r="M49" s="4"/>
+    </row>
+    <row r="51" spans="1:15" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I49" s="4" t="s">
+      <c r="I51" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A50" s="12" t="s">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A52" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B50" s="13" t="s">
+      <c r="B52" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C50" s="13" t="s">
+      <c r="C52" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D50" s="13" t="s">
+      <c r="D52" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E50" s="14" t="s">
+      <c r="E52" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F50" s="13" t="s">
+      <c r="F52" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G50" s="15" t="s">
+      <c r="G52" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I50" s="57" t="s">
+      <c r="I52" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="J50" s="16" t="s">
+      <c r="J52" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="K50" s="16" t="s">
+      <c r="K52" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="L50" s="16" t="s">
+      <c r="L52" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="M50" s="17" t="s">
+      <c r="M52" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="N50" s="16" t="s">
+      <c r="N52" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="O50" s="16" t="s">
+      <c r="O52" s="16" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="51" spans="1:15" ht="24" x14ac:dyDescent="0.25">
-      <c r="A51" s="59">
+    <row r="53" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+      <c r="A53" s="59">
         <v>1</v>
       </c>
-      <c r="B51" s="61" t="s">
+      <c r="B53" s="61" t="s">
         <v>74</v>
       </c>
-      <c r="C51" s="61" t="s">
+      <c r="C53" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="D51" s="61" t="s">
+      <c r="D53" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="E51" s="60" t="s">
+      <c r="E53" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F51" s="61"/>
-      <c r="G51" s="23" t="s">
+      <c r="F53" s="61"/>
+      <c r="G53" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="I51" s="58">
+      <c r="I53" s="58">
         <v>1</v>
       </c>
-      <c r="J51" s="4" t="s">
+      <c r="J53" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="K51" s="5" t="s">
+      <c r="K53" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="L51" s="56">
+      <c r="L53" s="56">
         <v>1415962923</v>
       </c>
-      <c r="M51" s="56">
+      <c r="M53" s="56">
         <v>1415962923</v>
       </c>
-      <c r="N51" s="4">
+      <c r="N53" s="4">
         <v>1</v>
       </c>
-      <c r="O51" s="4">
+      <c r="O53" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:15" ht="24" x14ac:dyDescent="0.25">
-      <c r="A52" s="18">
+    <row r="54" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+      <c r="A54" s="18">
         <v>2</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B54" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C54" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D52" s="4" t="s">
+      <c r="D54" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E52" s="58" t="s">
+      <c r="E54" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="F52" s="4"/>
-      <c r="G52" s="4"/>
-      <c r="I52" s="58">
+      <c r="F54" s="4"/>
+      <c r="G54" s="4"/>
+      <c r="I54" s="58">
         <v>2</v>
       </c>
-      <c r="J52" s="4" t="s">
+      <c r="J54" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="K52" s="5" t="s">
+      <c r="K54" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="L52" s="56">
+      <c r="L54" s="56">
         <v>1415962923</v>
       </c>
-      <c r="M52" s="56">
+      <c r="M54" s="56">
         <v>1415962923</v>
       </c>
-      <c r="N52" s="4">
+      <c r="N54" s="4">
         <v>2</v>
       </c>
-      <c r="O52" s="4">
+      <c r="O54" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A53" s="59">
+    <row r="55" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="A55" s="59">
         <v>3</v>
       </c>
-      <c r="B53" s="26" t="s">
+      <c r="B55" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="C53" s="27" t="s">
+      <c r="C55" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="D53" s="28" t="s">
+      <c r="D55" s="28" t="s">
         <v>24</v>
-      </c>
-      <c r="E53" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="F53" s="30"/>
-      <c r="G53" s="31"/>
-      <c r="I53" s="58"/>
-      <c r="L53" s="62"/>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A54" s="18">
-        <v>4</v>
-      </c>
-      <c r="B54" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="C54" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="D54" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="E54" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="F54" s="30"/>
-      <c r="G54" s="31"/>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A55" s="59">
-        <v>5</v>
-      </c>
-      <c r="B55" s="26" t="s">
-        <v>80</v>
-      </c>
-      <c r="C55" s="28" t="s">
-        <v>81</v>
-      </c>
-      <c r="D55" s="28" t="s">
-        <v>20</v>
       </c>
       <c r="E55" s="29" t="s">
         <v>21</v>
       </c>
       <c r="F55" s="30"/>
       <c r="G55" s="31"/>
+      <c r="I55" s="58"/>
+      <c r="L55" s="62"/>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" s="18">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B56" s="26" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C56" s="28" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D56" s="28" t="s">
         <v>20</v>
@@ -2550,448 +2580,459 @@
       </c>
       <c r="F56" s="30"/>
       <c r="G56" s="31"/>
-      <c r="I56" s="19"/>
-      <c r="J56" s="20"/>
-      <c r="K56" s="19"/>
-      <c r="L56" s="21"/>
-      <c r="M56" s="22"/>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="59">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B57" s="26" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C57" s="28" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="D57" s="28" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="E57" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="F57" s="30" t="s">
+      <c r="F57" s="30"/>
+      <c r="G57" s="31"/>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A58" s="18">
+        <v>6</v>
+      </c>
+      <c r="B58" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="C58" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="D58" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="E58" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="F58" s="30"/>
+      <c r="G58" s="31"/>
+      <c r="I58" s="19"/>
+      <c r="J58" s="20"/>
+      <c r="K58" s="19"/>
+      <c r="L58" s="21"/>
+      <c r="M58" s="22"/>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A59" s="59">
+        <v>7</v>
+      </c>
+      <c r="B59" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="C59" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="D59" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="E59" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="F59" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="G57" s="31" t="s">
+      <c r="G59" s="31" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="59" spans="1:15" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="1" t="s">
+    <row r="61" spans="1:15" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="60" spans="1:15" ht="24" x14ac:dyDescent="0.25">
-      <c r="A60" s="38" t="s">
+    <row r="62" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+      <c r="A62" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="B60" s="39" t="s">
+      <c r="B62" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="C60" s="63" t="s">
+      <c r="C62" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="D60" s="64"/>
-      <c r="E60" s="39" t="s">
+      <c r="D62" s="64"/>
+      <c r="E62" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="F60" s="39" t="s">
+      <c r="F62" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="G60" s="40" t="s">
+      <c r="G62" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="I60" s="48"/>
-      <c r="J60" s="48"/>
-      <c r="K60" s="48"/>
-      <c r="L60" s="48"/>
-    </row>
-    <row r="61" spans="1:15" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A61" s="41">
-        <v>1</v>
-      </c>
-      <c r="B61" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="C61" s="65" t="s">
-        <v>18</v>
-      </c>
-      <c r="D61" s="66"/>
-      <c r="E61" s="43" t="s">
-        <v>21</v>
-      </c>
-      <c r="F61" s="43" t="s">
-        <v>21</v>
-      </c>
-      <c r="G61" s="44"/>
-      <c r="I61" s="48"/>
-      <c r="J61" s="48"/>
-      <c r="K61" s="48"/>
-      <c r="L61" s="48"/>
-    </row>
-    <row r="62" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="45">
-        <v>2</v>
-      </c>
-      <c r="B62" s="34"/>
-      <c r="C62" s="67"/>
-      <c r="D62" s="68"/>
-      <c r="E62" s="46"/>
-      <c r="F62" s="46"/>
-      <c r="G62" s="47"/>
       <c r="I62" s="48"/>
       <c r="J62" s="48"/>
       <c r="K62" s="48"/>
       <c r="L62" s="48"/>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A63" s="41">
+        <v>1</v>
+      </c>
+      <c r="B63" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="C63" s="65" t="s">
+        <v>18</v>
+      </c>
+      <c r="D63" s="66"/>
+      <c r="E63" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="F63" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="G63" s="44"/>
       <c r="I63" s="48"/>
       <c r="J63" s="48"/>
       <c r="K63" s="48"/>
       <c r="L63" s="48"/>
     </row>
-    <row r="64" spans="1:15" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="1" t="s">
+    <row r="64" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="45">
+        <v>2</v>
+      </c>
+      <c r="B64" s="34"/>
+      <c r="C64" s="67"/>
+      <c r="D64" s="68"/>
+      <c r="E64" s="46"/>
+      <c r="F64" s="46"/>
+      <c r="G64" s="47"/>
+      <c r="I64" s="48"/>
+      <c r="J64" s="48"/>
+      <c r="K64" s="48"/>
+      <c r="L64" s="48"/>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I65" s="48"/>
+      <c r="J65" s="48"/>
+      <c r="K65" s="48"/>
+      <c r="L65" s="48"/>
+    </row>
+    <row r="66" spans="1:13" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="51" t="s">
+    <row r="67" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="B65" s="52" t="s">
+      <c r="B67" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="C65" s="69" t="s">
+      <c r="C67" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="D65" s="70"/>
-      <c r="E65" s="69" t="s">
+      <c r="D67" s="70"/>
+      <c r="E67" s="69" t="s">
         <v>33</v>
       </c>
-      <c r="F65" s="71"/>
-      <c r="G65" s="53" t="s">
+      <c r="F67" s="71"/>
+      <c r="G67" s="53" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="4">
+      <c r="M67" s="4"/>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A68" s="4">
         <v>1</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="C68" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E66" s="2" t="s">
+      <c r="E68" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G66" s="2" t="s">
+      <c r="G68" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="1" t="s">
+      <c r="M68" s="4"/>
+    </row>
+    <row r="70" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="51" t="s">
+      <c r="M70" s="4"/>
+    </row>
+    <row r="71" spans="1:13" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="B69" s="52" t="s">
+      <c r="B71" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="C69" s="69" t="s">
+      <c r="C71" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="D69" s="70"/>
-      <c r="E69" s="69" t="s">
+      <c r="D71" s="70"/>
+      <c r="E71" s="69" t="s">
         <v>36</v>
       </c>
-      <c r="F69" s="70"/>
-      <c r="G69" s="53" t="s">
+      <c r="F71" s="70"/>
+      <c r="G71" s="53" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="1" t="s">
+      <c r="M71" s="4"/>
+    </row>
+    <row r="76" spans="1:13" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="B75" s="6" t="s">
+      <c r="M76" s="4"/>
+    </row>
+    <row r="77" spans="1:13" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="B77" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C75" s="85" t="s">
+      <c r="C77" s="85" t="s">
         <v>38</v>
       </c>
-      <c r="D75" s="86"/>
-      <c r="E75" s="7" t="s">
+      <c r="D77" s="86"/>
+      <c r="E77" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F75" s="85" t="s">
+      <c r="F77" s="85" t="s">
         <v>39</v>
       </c>
-      <c r="G75" s="87"/>
-    </row>
-    <row r="76" spans="1:7" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="B76" s="8" t="s">
+      <c r="G77" s="87"/>
+      <c r="M77" s="4"/>
+    </row>
+    <row r="78" spans="1:13" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="B78" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C76" s="72"/>
-      <c r="D76" s="73"/>
-      <c r="E76" s="10" t="s">
+      <c r="C78" s="72"/>
+      <c r="D78" s="73"/>
+      <c r="E78" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F76" s="88" t="s">
+      <c r="F78" s="88" t="s">
         <v>40</v>
       </c>
-      <c r="G76" s="74"/>
-    </row>
-    <row r="77" spans="1:7" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="B77" s="8" t="s">
+      <c r="G78" s="74"/>
+      <c r="M78" s="4"/>
+    </row>
+    <row r="79" spans="1:13" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="B79" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C77" s="72"/>
-      <c r="D77" s="73"/>
-      <c r="E77" s="10" t="s">
+      <c r="C79" s="72"/>
+      <c r="D79" s="73"/>
+      <c r="E79" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F77" s="72"/>
-      <c r="G77" s="74"/>
-    </row>
-    <row r="78" spans="1:7" ht="24" x14ac:dyDescent="0.25">
-      <c r="B78" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C78" s="72" t="s">
-        <v>93</v>
-      </c>
-      <c r="D78" s="73"/>
-      <c r="E78" s="10"/>
-      <c r="F78" s="72"/>
-      <c r="G78" s="74"/>
-    </row>
-    <row r="79" spans="1:7" ht="24" x14ac:dyDescent="0.25">
-      <c r="B79" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C79" s="72" t="s">
-        <v>94</v>
-      </c>
-      <c r="D79" s="73"/>
-      <c r="E79" s="11"/>
       <c r="F79" s="72"/>
       <c r="G79" s="74"/>
-    </row>
-    <row r="80" spans="1:7" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="B80" s="75" t="s">
+      <c r="M79" s="4"/>
+    </row>
+    <row r="80" spans="1:13" ht="24" x14ac:dyDescent="0.25">
+      <c r="B80" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C80" s="72" t="s">
+        <v>93</v>
+      </c>
+      <c r="D80" s="73"/>
+      <c r="E80" s="10"/>
+      <c r="F80" s="72"/>
+      <c r="G80" s="74"/>
+      <c r="M80" s="4"/>
+    </row>
+    <row r="81" spans="1:14" ht="24" x14ac:dyDescent="0.25">
+      <c r="B81" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C81" s="72" t="s">
+        <v>94</v>
+      </c>
+      <c r="D81" s="73"/>
+      <c r="E81" s="11"/>
+      <c r="F81" s="72"/>
+      <c r="G81" s="74"/>
+      <c r="M81" s="4"/>
+    </row>
+    <row r="82" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="B82" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="C80" s="76"/>
-      <c r="D80" s="76"/>
-      <c r="E80" s="76"/>
-      <c r="F80" s="76"/>
-      <c r="G80" s="77"/>
-    </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B81" s="78"/>
-      <c r="C81" s="79"/>
-      <c r="D81" s="79"/>
-      <c r="E81" s="79"/>
-      <c r="F81" s="79"/>
-      <c r="G81" s="80"/>
-    </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B82" s="81"/>
-      <c r="C82" s="79"/>
-      <c r="D82" s="79"/>
-      <c r="E82" s="79"/>
-      <c r="F82" s="79"/>
-      <c r="G82" s="80"/>
-    </row>
-    <row r="83" spans="1:14" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B83" s="82"/>
-      <c r="C83" s="83"/>
-      <c r="D83" s="83"/>
-      <c r="E83" s="83"/>
-      <c r="F83" s="83"/>
-      <c r="G83" s="84"/>
+      <c r="C82" s="76"/>
+      <c r="D82" s="76"/>
+      <c r="E82" s="76"/>
+      <c r="F82" s="76"/>
+      <c r="G82" s="77"/>
+      <c r="M82" s="4"/>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B83" s="78"/>
+      <c r="C83" s="79"/>
+      <c r="D83" s="79"/>
+      <c r="E83" s="79"/>
+      <c r="F83" s="79"/>
+      <c r="G83" s="80"/>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B84" s="81"/>
+      <c r="C84" s="79"/>
+      <c r="D84" s="79"/>
+      <c r="E84" s="79"/>
+      <c r="F84" s="79"/>
+      <c r="G84" s="80"/>
     </row>
     <row r="85" spans="1:14" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="1" t="s">
+      <c r="B85" s="82"/>
+      <c r="C85" s="83"/>
+      <c r="D85" s="83"/>
+      <c r="E85" s="83"/>
+      <c r="F85" s="83"/>
+      <c r="G85" s="84"/>
+    </row>
+    <row r="87" spans="1:14" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I85" s="4" t="s">
+      <c r="I87" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A86" s="12" t="s">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A88" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B86" s="13" t="s">
+      <c r="B88" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C86" s="13" t="s">
+      <c r="C88" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D86" s="13" t="s">
+      <c r="D88" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E86" s="14" t="s">
+      <c r="E88" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F86" s="13" t="s">
+      <c r="F88" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G86" s="15" t="s">
+      <c r="G88" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I86" s="57" t="s">
+      <c r="I88" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="J86" s="16" t="s">
+      <c r="J88" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="K86" s="16" t="s">
+      <c r="K88" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="L86" s="17" t="s">
+      <c r="L88" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="M86" s="17" t="s">
+      <c r="M88" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="N86" s="16" t="s">
+      <c r="N88" s="16" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A87" s="59">
-        <v>1</v>
-      </c>
-      <c r="B87" s="61" t="s">
-        <v>95</v>
-      </c>
-      <c r="C87" s="61" t="s">
-        <v>18</v>
-      </c>
-      <c r="D87" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="E87" s="60" t="s">
-        <v>21</v>
-      </c>
-      <c r="F87" s="61"/>
-      <c r="G87" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="I87" s="58">
-        <v>1</v>
-      </c>
-      <c r="J87" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="K87" s="56">
-        <v>1415962923</v>
-      </c>
-      <c r="L87" s="56">
-        <v>1415962923</v>
-      </c>
-      <c r="M87" s="5">
-        <v>1</v>
-      </c>
-      <c r="N87" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:14" ht="24" x14ac:dyDescent="0.25">
-      <c r="A88" s="18">
-        <v>2</v>
-      </c>
-      <c r="B88" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C88" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D88" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E88" s="58" t="s">
-        <v>21</v>
-      </c>
-      <c r="F88" s="4"/>
-      <c r="G88" s="4"/>
-      <c r="I88" s="58">
-        <v>2</v>
-      </c>
-      <c r="J88" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="K88" s="56">
-        <v>1415962923</v>
-      </c>
-      <c r="L88" s="56">
-        <v>1415962923</v>
-      </c>
-      <c r="M88" s="5">
-        <v>1</v>
-      </c>
-      <c r="N88" s="4">
-        <v>2</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" s="59">
-        <v>3</v>
-      </c>
-      <c r="B89" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="C89" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="D89" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B89" s="61" t="s">
+        <v>95</v>
+      </c>
+      <c r="C89" s="61" t="s">
+        <v>18</v>
+      </c>
+      <c r="D89" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="E89" s="29" t="s">
+      <c r="E89" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F89" s="30"/>
-      <c r="G89" s="31"/>
-    </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F89" s="61"/>
+      <c r="G89" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="I89" s="58">
+        <v>1</v>
+      </c>
+      <c r="J89" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="K89" s="56">
+        <v>1415962923</v>
+      </c>
+      <c r="L89" s="56">
+        <v>1415962923</v>
+      </c>
+      <c r="M89" s="5">
+        <v>1</v>
+      </c>
+      <c r="N89" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" ht="24" x14ac:dyDescent="0.25">
       <c r="A90" s="18">
-        <v>4</v>
-      </c>
-      <c r="B90" s="26" t="s">
-        <v>80</v>
-      </c>
-      <c r="C90" s="28" t="s">
-        <v>81</v>
-      </c>
-      <c r="D90" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="E90" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D90" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E90" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="F90" s="30"/>
-      <c r="G90" s="31"/>
+      <c r="F90" s="4"/>
+      <c r="G90" s="4"/>
+      <c r="I90" s="58">
+        <v>2</v>
+      </c>
+      <c r="J90" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="K90" s="56">
+        <v>1415962923</v>
+      </c>
+      <c r="L90" s="56">
+        <v>1415962923</v>
+      </c>
+      <c r="M90" s="5">
+        <v>1</v>
+      </c>
+      <c r="N90" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" s="59">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B91" s="26" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C91" s="28" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D91" s="28" t="s">
         <v>20</v>
@@ -3004,13 +3045,13 @@
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" s="18">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B92" s="26" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="C92" s="28" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="D92" s="28" t="s">
         <v>20</v>
@@ -3021,248 +3062,368 @@
       <c r="F92" s="30"/>
       <c r="G92" s="31"/>
     </row>
-    <row r="94" spans="1:14" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="1" t="s">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A93" s="59">
+        <v>5</v>
+      </c>
+      <c r="B93" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="C93" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="D93" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="E93" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="F93" s="30"/>
+      <c r="G93" s="31"/>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A94" s="18">
+        <v>6</v>
+      </c>
+      <c r="B94" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="C94" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="D94" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="E94" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="F94" s="30"/>
+      <c r="G94" s="31"/>
+    </row>
+    <row r="96" spans="1:14" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="95" spans="1:14" ht="24" x14ac:dyDescent="0.25">
-      <c r="A95" s="38" t="s">
+    <row r="97" spans="1:13" ht="24" x14ac:dyDescent="0.25">
+      <c r="A97" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="B95" s="39" t="s">
+      <c r="B97" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="C95" s="63" t="s">
+      <c r="C97" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="D95" s="64"/>
-      <c r="E95" s="39" t="s">
+      <c r="D97" s="64"/>
+      <c r="E97" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="F95" s="39" t="s">
+      <c r="F97" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="G95" s="40" t="s">
+      <c r="G97" s="40" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A96" s="41">
+    <row r="98" spans="1:13" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A98" s="41">
         <v>1</v>
       </c>
-      <c r="B96" s="42" t="s">
+      <c r="B98" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="C96" s="65" t="s">
+      <c r="C98" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="D96" s="66"/>
-      <c r="E96" s="43" t="s">
+      <c r="D98" s="66"/>
+      <c r="E98" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="F96" s="43" t="s">
+      <c r="F98" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="G96" s="44"/>
-    </row>
-    <row r="97" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="45">
+      <c r="G98" s="44"/>
+    </row>
+    <row r="99" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="45">
         <v>2</v>
       </c>
-      <c r="B97" s="34"/>
-      <c r="C97" s="67"/>
-      <c r="D97" s="68"/>
-      <c r="E97" s="46"/>
-      <c r="F97" s="46"/>
-      <c r="G97" s="47"/>
-    </row>
-    <row r="99" spans="1:7" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="1" t="s">
+      <c r="B99" s="34"/>
+      <c r="C99" s="67"/>
+      <c r="D99" s="68"/>
+      <c r="E99" s="46"/>
+      <c r="F99" s="46"/>
+      <c r="G99" s="47"/>
+      <c r="M99" s="4"/>
+    </row>
+    <row r="101" spans="1:13" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="51" t="s">
+      <c r="M101" s="4"/>
+    </row>
+    <row r="102" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="B100" s="52" t="s">
+      <c r="B102" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="C100" s="69" t="s">
+      <c r="C102" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="D100" s="70"/>
-      <c r="E100" s="69" t="s">
+      <c r="D102" s="70"/>
+      <c r="E102" s="69" t="s">
         <v>33</v>
       </c>
-      <c r="F100" s="71"/>
-      <c r="G100" s="53" t="s">
+      <c r="F102" s="71"/>
+      <c r="G102" s="53" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A101" s="4">
+      <c r="M102" s="4"/>
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A103" s="4">
         <v>1</v>
       </c>
-      <c r="C101" s="2" t="s">
+      <c r="C103" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E101" s="2" t="s">
+      <c r="E103" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G101" s="2" t="s">
+      <c r="G103" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A102" s="4">
+      <c r="M103" s="4"/>
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A104" s="4">
         <v>2</v>
       </c>
-      <c r="C102" s="2" t="s">
+      <c r="C104" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E102" s="2" t="s">
+      <c r="E104" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G102" s="2" t="s">
+      <c r="G104" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="103" spans="1:7" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="1" t="s">
+      <c r="M104" s="4"/>
+    </row>
+    <row r="105" spans="1:13" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="104" spans="1:7" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="51" t="s">
+      <c r="M105" s="4"/>
+    </row>
+    <row r="106" spans="1:13" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="B104" s="52" t="s">
+      <c r="B106" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="C104" s="69" t="s">
+      <c r="C106" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="D104" s="70"/>
-      <c r="E104" s="69" t="s">
+      <c r="D106" s="70"/>
+      <c r="E106" s="69" t="s">
         <v>36</v>
       </c>
-      <c r="F104" s="70"/>
-      <c r="G104" s="53" t="s">
+      <c r="F106" s="70"/>
+      <c r="G106" s="53" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="116" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C116" s="90" t="s">
+      <c r="M106" s="4"/>
+    </row>
+    <row r="118" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B118" s="4"/>
+      <c r="C118" s="90" t="s">
         <v>41</v>
       </c>
-      <c r="F116" s="89" t="s">
+      <c r="F118" s="89" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="117" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C117" s="9" t="s">
+      <c r="G118" s="4"/>
+      <c r="M118" s="4"/>
+    </row>
+    <row r="119" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B119" s="4"/>
+      <c r="C119" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="F117" s="9" t="s">
+      <c r="F119" s="9" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="118" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C118" s="9" t="s">
+      <c r="G119" s="4"/>
+      <c r="M119" s="4"/>
+    </row>
+    <row r="120" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B120" s="4"/>
+      <c r="C120" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="F118" s="9" t="s">
+      <c r="F120" s="9" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="119" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C119" s="9" t="s">
+      <c r="G120" s="4"/>
+      <c r="M120" s="4"/>
+    </row>
+    <row r="121" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B121" s="4"/>
+      <c r="C121" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="F119" s="9" t="s">
+      <c r="F121" s="9" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="120" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C120" s="9" t="s">
+      <c r="G121" s="4"/>
+      <c r="M121" s="4"/>
+    </row>
+    <row r="122" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B122" s="4"/>
+      <c r="C122" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="F120" s="9" t="s">
+      <c r="F122" s="9" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="121" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C121" s="9" t="s">
+      <c r="G122" s="4"/>
+      <c r="M122" s="4"/>
+    </row>
+    <row r="123" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B123" s="4"/>
+      <c r="C123" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="F121" s="9" t="s">
+      <c r="F123" s="9" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="122" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C122" s="9" t="s">
+      <c r="G123" s="4"/>
+      <c r="M123" s="4"/>
+    </row>
+    <row r="124" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B124" s="4"/>
+      <c r="C124" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="F122" s="9" t="s">
+      <c r="F124" s="9" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="123" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C123" s="9" t="s">
+      <c r="G124" s="4"/>
+      <c r="M124" s="4"/>
+    </row>
+    <row r="125" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B125" s="4"/>
+      <c r="C125" s="9" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="124" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C124" s="9" t="s">
+      <c r="G125" s="4"/>
+      <c r="M125" s="4"/>
+    </row>
+    <row r="126" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B126" s="4"/>
+      <c r="C126" s="9" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="125" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C125" s="9" t="s">
+      <c r="G126" s="4"/>
+      <c r="M126" s="4"/>
+    </row>
+    <row r="127" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B127" s="4"/>
+      <c r="C127" s="9" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="128" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D128" s="89" t="s">
+      <c r="G127" s="4"/>
+      <c r="M127" s="4"/>
+    </row>
+    <row r="130" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B130" s="4"/>
+      <c r="D130" s="89" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="129" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D129" s="9" t="s">
+      <c r="G130" s="4"/>
+      <c r="M130" s="4"/>
+    </row>
+    <row r="131" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B131" s="4"/>
+      <c r="C131" s="4"/>
+      <c r="D131" s="9" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="130" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D130" s="9" t="s">
+      <c r="E131" s="4"/>
+      <c r="F131" s="4"/>
+      <c r="G131" s="4"/>
+      <c r="M131" s="4"/>
+    </row>
+    <row r="132" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B132" s="4"/>
+      <c r="C132" s="4"/>
+      <c r="D132" s="9" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="131" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D131" s="9" t="s">
+      <c r="E132" s="4"/>
+      <c r="F132" s="4"/>
+      <c r="G132" s="4"/>
+      <c r="M132" s="4"/>
+    </row>
+    <row r="133" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B133" s="4"/>
+      <c r="C133" s="4"/>
+      <c r="D133" s="9" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="132" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D132" s="9" t="s">
+      <c r="E133" s="4"/>
+      <c r="F133" s="4"/>
+      <c r="G133" s="4"/>
+      <c r="M133" s="4"/>
+    </row>
+    <row r="134" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B134" s="4"/>
+      <c r="C134" s="4"/>
+      <c r="D134" s="9" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="133" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D133" s="9" t="s">
+      <c r="E134" s="4"/>
+      <c r="F134" s="4"/>
+      <c r="G134" s="4"/>
+      <c r="M134" s="4"/>
+    </row>
+    <row r="135" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B135" s="4"/>
+      <c r="C135" s="4"/>
+      <c r="D135" s="9" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="134" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D134" s="9" t="s">
+      <c r="E135" s="4"/>
+      <c r="F135" s="4"/>
+      <c r="G135" s="4"/>
+      <c r="M135" s="4"/>
+    </row>
+    <row r="136" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B136" s="4"/>
+      <c r="C136" s="4"/>
+      <c r="D136" s="9" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="135" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D135" s="9" t="s">
+      <c r="E136" s="4"/>
+      <c r="F136" s="4"/>
+      <c r="G136" s="4"/>
+      <c r="M136" s="4"/>
+    </row>
+    <row r="137" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B137" s="4"/>
+      <c r="C137" s="4"/>
+      <c r="D137" s="9" t="s">
         <v>57</v>
       </c>
+      <c r="E137" s="4"/>
+      <c r="F137" s="4"/>
+      <c r="G137" s="4"/>
+      <c r="M137" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="57">
@@ -3278,51 +3439,51 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="B7:G7"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
     <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:F32"/>
     <mergeCell ref="C41:D41"/>
     <mergeCell ref="F41:G41"/>
     <mergeCell ref="C42:D42"/>
     <mergeCell ref="F42:G42"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="E35:F35"/>
     <mergeCell ref="C43:D43"/>
     <mergeCell ref="F43:G43"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="E69:F69"/>
-    <mergeCell ref="B44:G44"/>
-    <mergeCell ref="B45:G47"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="E71:F71"/>
+    <mergeCell ref="B46:G46"/>
+    <mergeCell ref="B47:G49"/>
     <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="E65:F65"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="F75:G75"/>
-    <mergeCell ref="C76:D76"/>
-    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="E67:F67"/>
     <mergeCell ref="C77:D77"/>
     <mergeCell ref="F77:G77"/>
-    <mergeCell ref="C104:D104"/>
-    <mergeCell ref="E104:F104"/>
     <mergeCell ref="C78:D78"/>
     <mergeCell ref="F78:G78"/>
     <mergeCell ref="C79:D79"/>
     <mergeCell ref="F79:G79"/>
-    <mergeCell ref="B80:G80"/>
-    <mergeCell ref="B81:G83"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="C106:D106"/>
+    <mergeCell ref="E106:F106"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="F80:G80"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="F81:G81"/>
+    <mergeCell ref="B82:G82"/>
+    <mergeCell ref="B83:G85"/>
     <mergeCell ref="C97:D97"/>
-    <mergeCell ref="C100:D100"/>
-    <mergeCell ref="E100:F100"/>
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="C99:D99"/>
+    <mergeCell ref="C102:D102"/>
+    <mergeCell ref="E102:F102"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L14" r:id="rId1"/>

</xml_diff>